<commit_message>
Well T6 python and CORE changes
</commit_message>
<xml_diff>
--- a/CORE/CORE.xlsx
+++ b/CORE/CORE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angelica\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C60C2BE-BD94-4A6E-9814-D0844730A2F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FBD64B-BF5F-4CBF-B07D-6748C6983107}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CF367FB8-77F3-451A-B253-26A736045F64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CF367FB8-77F3-451A-B253-26A736045F64}"/>
   </bookViews>
   <sheets>
     <sheet name="Gamma" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,6 +315,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -633,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDD81CC-306E-4459-8DB1-102871A6218E}">
   <dimension ref="A1:O486"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="111" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157:C363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +675,7 @@
         <v>70.423657889589776</v>
       </c>
       <c r="C2" s="4">
-        <v>83.209877541533558</v>
+        <v>83.209877541533601</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -2832,2898 +2838,2898 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="32">
+      <c r="A157" s="33">
         <v>3376.9999999999995</v>
       </c>
       <c r="B157" s="38">
         <v>20.927710769465801</v>
       </c>
       <c r="C157" s="38">
-        <v>83.099907999858829</v>
+        <v>69.719889599830594</v>
       </c>
       <c r="D157" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="3">
+      <c r="A158" s="13">
         <v>3377.5383495145625</v>
       </c>
       <c r="B158" s="4">
         <v>45.357685784253754</v>
       </c>
       <c r="C158" s="4">
-        <v>88.146820344515675</v>
+        <v>75.776184413418804</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="3">
+      <c r="A159" s="13">
         <v>3378.0766990291258</v>
       </c>
       <c r="B159" s="4">
         <v>60.58676588916471</v>
       </c>
       <c r="C159" s="4">
-        <v>91.292948506035202</v>
+        <v>79.55153820724226</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="3">
+      <c r="A160" s="13">
         <v>3378.6150485436888</v>
       </c>
       <c r="B160" s="4">
         <v>69.069634405000414</v>
       </c>
       <c r="C160" s="4">
-        <v>93.045397855850624</v>
+        <v>81.654477427020751</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="3">
+      <c r="A161" s="13">
         <v>3379.1533980582522</v>
       </c>
       <c r="B161" s="4">
         <v>68.334897761896528</v>
       </c>
       <c r="C161" s="4">
-        <v>92.893610904291805</v>
+        <v>81.472333085150154</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="3">
+      <c r="A162" s="13">
         <v>3379.6917475728151</v>
       </c>
       <c r="B162" s="4">
         <v>59.7184474449205</v>
       </c>
       <c r="C162" s="4">
-        <v>91.113565306801632</v>
+        <v>79.336278368161942</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="3">
+      <c r="A163" s="13">
         <v>3380.230097087378</v>
       </c>
       <c r="B163" s="4">
         <v>54.241333100630548</v>
       </c>
       <c r="C163" s="4">
-        <v>89.982065336762304</v>
+        <v>77.978478404114753</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="3">
+      <c r="A164" s="13">
         <v>3380.7684466019414</v>
       </c>
       <c r="B164" s="4">
         <v>60.491213631037951</v>
       </c>
       <c r="C164" s="4">
-        <v>91.273208663042823</v>
+        <v>79.527850395651399</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="3">
+      <c r="A165" s="13">
         <v>3381.3067961165043</v>
       </c>
       <c r="B165" s="4">
         <v>59.765735154255026</v>
       </c>
       <c r="C165" s="4">
-        <v>91.12333432718934</v>
+        <v>79.348001192627208</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="3">
+      <c r="A166" s="13">
         <v>3381.8451456310677</v>
       </c>
       <c r="B166" s="4">
         <v>61.893879318115488</v>
       </c>
       <c r="C166" s="4">
-        <v>91.562980992619629</v>
+        <v>79.875577191143549</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="3">
+      <c r="A167" s="13">
         <v>3382.3834951456306</v>
       </c>
       <c r="B167" s="4">
         <v>77.018128960306655</v>
       </c>
       <c r="C167" s="4">
-        <v>94.687452555797307</v>
+        <v>83.624943066956774</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="3">
+      <c r="A168" s="13">
         <v>3382.9218446601935</v>
       </c>
       <c r="B168" s="4">
         <v>71.674609776005056</v>
       </c>
       <c r="C168" s="4">
-        <v>93.583551593195523</v>
+        <v>82.30026191183461</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="3">
+      <c r="A169" s="13">
         <v>3383.4601941747569</v>
       </c>
       <c r="B169" s="4">
         <v>57.247073913328236</v>
       </c>
       <c r="C169" s="4">
-        <v>90.603011956775632</v>
+        <v>78.723614348130752</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="3">
+      <c r="A170" s="13">
         <v>3383.9985436893198</v>
       </c>
       <c r="B170" s="4">
         <v>60.920743769999582</v>
       </c>
       <c r="C170" s="4">
-        <v>91.361943954806947</v>
+        <v>79.634332745768347</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="3">
+      <c r="A171" s="13">
         <v>3384.5368932038832</v>
       </c>
       <c r="B171" s="4">
         <v>56.77950087250499</v>
       </c>
       <c r="C171" s="4">
-        <v>90.506417500566357</v>
+        <v>78.60770100067964</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="3">
+      <c r="A172" s="13">
         <v>3385.0752427184461</v>
       </c>
       <c r="B172" s="4">
         <v>58.11539903699645</v>
       </c>
       <c r="C172" s="4">
-        <v>90.782396535890598</v>
+        <v>78.938875843068715</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="3">
+      <c r="A173" s="13">
         <v>3385.6135922330095</v>
       </c>
       <c r="B173" s="4">
         <v>62.790989177324391</v>
       </c>
       <c r="C173" s="4">
-        <v>91.748312120474395</v>
+        <v>80.097974544569283</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="3">
+      <c r="A174" s="13">
         <v>3386.1519417475724</v>
       </c>
       <c r="B174" s="4">
         <v>63.191767977865467</v>
       </c>
       <c r="C174" s="4">
-        <v>91.831107762905617</v>
+        <v>80.197329315486741</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="3">
+      <c r="A175" s="13">
         <v>3386.6902912621354</v>
       </c>
       <c r="B175" s="4">
         <v>53.640198296939069</v>
       </c>
       <c r="C175" s="4">
-        <v>89.857878772522383</v>
+        <v>77.829454527026854</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="3">
+      <c r="A176" s="13">
         <v>3387.2286407766987</v>
       </c>
       <c r="B176" s="4">
         <v>63.726121900122848</v>
       </c>
       <c r="C176" s="4">
-        <v>91.941498273130208</v>
+        <v>80.329797927756246</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="3">
+      <c r="A177" s="13">
         <v>3387.7669902912617</v>
       </c>
       <c r="B177" s="4">
         <v>62.724188257618195</v>
       </c>
       <c r="C177" s="4">
-        <v>91.73451192681496</v>
+        <v>80.081414312177941</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="3">
+      <c r="A178" s="13">
         <v>3388.305339805825</v>
       </c>
       <c r="B178" s="4">
         <v>35.672520943338967</v>
       </c>
       <c r="C178" s="4">
-        <v>86.145992346694925</v>
+        <v>73.375190816033893</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="3">
+      <c r="A179" s="13">
         <v>3388.843689320388</v>
       </c>
       <c r="B179" s="4">
         <v>22.714458366869884</v>
       </c>
       <c r="C179" s="4">
-        <v>83.469026613392657</v>
+        <v>70.1628319360712</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="3">
+      <c r="A180" s="13">
         <v>3389.3820388349509</v>
       </c>
       <c r="B180" s="4">
         <v>23.649584410244309</v>
       </c>
       <c r="C180" s="4">
-        <v>83.662211386167087</v>
+        <v>70.394653663400504</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="3">
+      <c r="A181" s="13">
         <v>3389.9203883495143</v>
       </c>
       <c r="B181" s="4">
         <v>53.373021335810371</v>
       </c>
       <c r="C181" s="4">
-        <v>89.802683517410088</v>
+        <v>77.763220220892094</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="3">
+      <c r="A182" s="13">
         <v>3390.4587378640772</v>
       </c>
       <c r="B182" s="4">
         <v>69.537227484095723</v>
       </c>
       <c r="C182" s="4">
-        <v>93.141996451704031</v>
+        <v>81.770395742044826</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="3">
+      <c r="A183" s="13">
         <v>3390.9970873786406</v>
       </c>
       <c r="B183" s="4">
         <v>66.33109727112749</v>
       </c>
       <c r="C183" s="4">
-        <v>92.479652010475093</v>
+        <v>80.975582412570105</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="3">
+      <c r="A184" s="13">
         <v>3391.5354368932035</v>
       </c>
       <c r="B184" s="4">
         <v>56.044770908825129</v>
       </c>
       <c r="C184" s="4">
-        <v>90.354631928888921</v>
+        <v>78.425558314666702</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="3">
+      <c r="A185" s="13">
         <v>3392.0737864077664</v>
       </c>
       <c r="B185" s="4">
         <v>52.103917411601081</v>
       </c>
       <c r="C185" s="4">
-        <v>89.540503295863914</v>
+        <v>77.448603955036702</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="3">
+      <c r="A186" s="13">
         <v>3392.6121359223298</v>
       </c>
       <c r="B186" s="4">
         <v>52.571463734728219</v>
       </c>
       <c r="C186" s="4">
-        <v>89.637092232547687</v>
+        <v>77.564510679057221</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="3">
+      <c r="A187" s="13">
         <v>3393.1504854368927</v>
       </c>
       <c r="B187" s="4">
         <v>53.840554300089458</v>
       </c>
       <c r="C187" s="4">
-        <v>89.899269694331082</v>
+        <v>77.87912363319731</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="3">
+      <c r="A188" s="13">
         <v>3393.6888349514561</v>
       </c>
       <c r="B188" s="4">
         <v>52.838660734128986</v>
       </c>
       <c r="C188" s="4">
-        <v>89.692291627304101</v>
+        <v>77.630749952764944</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="3">
+      <c r="A189" s="13">
         <v>3394.227184466019</v>
       </c>
       <c r="B189" s="4">
         <v>57.8482287552918</v>
       </c>
       <c r="C189" s="4">
-        <v>90.727202660659685</v>
+        <v>78.872643192791614</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="3">
+      <c r="A190" s="13">
         <v>3394.7655339805819</v>
       </c>
       <c r="B190" s="4">
         <v>57.447443275326691</v>
       </c>
       <c r="C190" s="4">
-        <v>90.644405638347095</v>
+        <v>78.773286766016525</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="3">
+      <c r="A191" s="13">
         <v>3395.3038834951453</v>
       </c>
       <c r="B191" s="4">
         <v>55.911175748836762</v>
       </c>
       <c r="C191" s="4">
-        <v>90.327032921451405</v>
+        <v>78.392439505741663</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="3">
+      <c r="A192" s="13">
         <v>3395.8422330097083</v>
       </c>
       <c r="B192" s="4">
         <v>54.976076423158453</v>
       </c>
       <c r="C192" s="4">
-        <v>90.133853668202477</v>
+        <v>78.160624401842995</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="3">
+      <c r="A193" s="13">
         <v>3396.3805825242716</v>
       </c>
       <c r="B193" s="4">
         <v>55.577231265122009</v>
       </c>
       <c r="C193" s="4">
-        <v>90.25804437208653</v>
+        <v>78.309653246503842</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="3">
+      <c r="A194" s="13">
         <v>3396.9189320388346</v>
       </c>
       <c r="B194" s="4">
         <v>56.979910311047604</v>
       </c>
       <c r="C194" s="4">
-        <v>90.547819461426087</v>
+        <v>78.65738335371131</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="3">
+      <c r="A195" s="13">
         <v>3397.4572815533975</v>
       </c>
       <c r="B195" s="4">
         <v>60.920763808271658</v>
       </c>
       <c r="C195" s="4">
-        <v>91.361948094451094</v>
+        <v>79.634337713341296</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="3">
+      <c r="A196" s="13">
         <v>3397.9956310679609</v>
       </c>
       <c r="B196" s="4">
         <v>60.186007126895696</v>
       </c>
       <c r="C196" s="4">
-        <v>91.210157003248128</v>
+        <v>79.452188403897765</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="3">
+      <c r="A197" s="13">
         <v>3398.5339805825238</v>
       </c>
       <c r="B197" s="4">
         <v>52.304286773599529</v>
       </c>
       <c r="C197" s="4">
-        <v>89.581896977435377</v>
+        <v>77.498276372922462</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="3">
+      <c r="A198" s="13">
         <v>3399.0723300970872</v>
       </c>
       <c r="B198" s="4">
         <v>55.844394867402649</v>
       </c>
       <c r="C198" s="4">
-        <v>90.313236867436075</v>
+        <v>78.375884240923284</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="3">
+      <c r="A199" s="13">
         <v>3399.6106796116501</v>
       </c>
       <c r="B199" s="4">
         <v>52.237499212741398</v>
       </c>
       <c r="C199" s="4">
-        <v>89.568099543538693</v>
+        <v>77.481719452246438</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="3">
+      <c r="A200" s="13">
         <v>3400.149029126213</v>
       </c>
       <c r="B200" s="4">
         <v>54.441715821477068</v>
       </c>
       <c r="C200" s="4">
-        <v>90.023461778096518</v>
+        <v>78.028154133715816</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="3">
+      <c r="A201" s="13">
         <v>3400.6873786407764</v>
       </c>
       <c r="B201" s="4">
         <v>63.659307621568601</v>
       </c>
       <c r="C201" s="4">
-        <v>91.927695319707993</v>
+        <v>80.313234383649586</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="3">
+      <c r="A202" s="13">
         <v>3401.2257281553393</v>
       </c>
       <c r="B202" s="4">
         <v>71.006674052607394</v>
       </c>
       <c r="C202" s="4">
-        <v>93.445564835296153</v>
+        <v>82.134677802355384</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="3">
+      <c r="A203" s="13">
         <v>3401.7640776699027</v>
       </c>
       <c r="B203" s="4">
         <v>66.26430303084534</v>
       </c>
       <c r="C203" s="4">
-        <v>92.465853196697026</v>
+        <v>80.959023836036422</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="3">
+      <c r="A204" s="13">
         <v>3402.3024271844656</v>
       </c>
       <c r="B204" s="4">
         <v>61.922677412504228</v>
       </c>
       <c r="C204" s="4">
-        <v>91.568930301122208</v>
+        <v>79.882716361346638</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="3">
+      <c r="A205" s="13">
         <v>3402.8407766990285</v>
       </c>
       <c r="B205" s="4">
         <v>56.645912391940648</v>
       </c>
       <c r="C205" s="4">
-        <v>90.47881987301021</v>
+        <v>78.574583847612246</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="3">
+      <c r="A206" s="13">
         <v>3403.3791262135919</v>
       </c>
       <c r="B206" s="4">
         <v>49.832893203735175</v>
       </c>
       <c r="C206" s="4">
-        <v>89.071339487765272</v>
+        <v>76.885607385318309</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="3">
+      <c r="A207" s="13">
         <v>3403.9174757281548</v>
       </c>
       <c r="B207" s="4">
         <v>46.29279846878012</v>
       </c>
       <c r="C207" s="4">
-        <v>88.340002357527339</v>
+        <v>76.008002829032804</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="3">
+      <c r="A208" s="13">
         <v>3404.4558252427182</v>
       </c>
       <c r="B208" s="4">
         <v>44.890119422854539</v>
       </c>
       <c r="C208" s="4">
-        <v>88.050227268187783</v>
+        <v>75.660272721825336</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="3">
+      <c r="A209" s="13">
         <v>3404.9941747572811</v>
       </c>
       <c r="B209" s="4">
         <v>52.972229176421251</v>
       </c>
       <c r="C209" s="4">
-        <v>89.71988511521613</v>
+        <v>77.663862138259361</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="3">
+      <c r="A210" s="13">
         <v>3405.5325242718441</v>
       </c>
       <c r="B210" s="4">
         <v>56.979896952199553</v>
       </c>
       <c r="C210" s="4">
-        <v>90.547816701663351</v>
+        <v>78.657380041996007</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="3">
+      <c r="A211" s="13">
         <v>3406.0708737864074</v>
       </c>
       <c r="B211" s="4">
         <v>62.123040095078657</v>
       </c>
       <c r="C211" s="4">
-        <v>91.610322602812289</v>
+        <v>79.932387123374752</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="3">
+      <c r="A212" s="13">
         <v>3406.6092233009704</v>
       </c>
       <c r="B212" s="4">
         <v>59.317675323803449</v>
       </c>
       <c r="C212" s="4">
-        <v>91.030771044251793</v>
+        <v>79.236925253102157</v>
       </c>
       <c r="D212" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="3">
+      <c r="A213" s="13">
         <v>3407.1475728155337</v>
       </c>
       <c r="B213" s="4">
         <v>53.372987938690244</v>
       </c>
       <c r="C213" s="4">
-        <v>89.802676618003204</v>
+        <v>77.763211941603828</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="3">
+      <c r="A214" s="13">
         <v>3407.6859223300967</v>
       </c>
       <c r="B214" s="4">
         <v>55.643998787708071</v>
       </c>
       <c r="C214" s="4">
-        <v>90.27183766633911</v>
+        <v>78.326205199606918</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="3">
+      <c r="A215" s="13">
         <v>3408.2242718446596</v>
       </c>
       <c r="B215" s="4">
         <v>55.844394867402642</v>
       </c>
       <c r="C215" s="4">
-        <v>90.313236867436075</v>
+        <v>78.375884240923284</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="3">
+      <c r="A216" s="13">
         <v>3408.762621359223</v>
       </c>
       <c r="B216" s="4">
         <v>53.9741427806538</v>
       </c>
       <c r="C216" s="4">
-        <v>89.926867321887244</v>
+        <v>77.91224078626469</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="3">
+      <c r="A217" s="13">
         <v>3409.3009708737859</v>
       </c>
       <c r="B217" s="4">
         <v>53.573377338960782</v>
       </c>
       <c r="C217" s="4">
-        <v>89.844074439218787</v>
+        <v>77.81288932706255</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="3">
+      <c r="A218" s="13">
         <v>3409.8393203883493</v>
       </c>
       <c r="B218" s="4">
         <v>58.31578175784297</v>
       </c>
       <c r="C218" s="4">
-        <v>90.823792977224812</v>
+        <v>78.988551572669792</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="3">
+      <c r="A219" s="13">
         <v>3410.3776699029122</v>
       </c>
       <c r="B219" s="4">
         <v>69.336811366129098</v>
       </c>
       <c r="C219" s="4">
-        <v>93.100593110962933</v>
+        <v>81.720711733155497</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" s="3">
+      <c r="A220" s="13">
         <v>3410.9160194174751</v>
       </c>
       <c r="B220" s="4">
         <v>78.487602246514442</v>
       </c>
       <c r="C220" s="4">
-        <v>94.991026458914945</v>
+        <v>83.98923175069794</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="3">
+      <c r="A221" s="13">
         <v>3411.4543689320385</v>
       </c>
       <c r="B221" s="4">
         <v>69.537187407551585</v>
       </c>
       <c r="C221" s="4">
-        <v>93.141988172415779</v>
+        <v>81.770385806898929</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="3">
+      <c r="A222" s="13">
         <v>3411.9927184466014</v>
       </c>
       <c r="B222" s="4">
         <v>68.134515041050037</v>
       </c>
       <c r="C222" s="4">
-        <v>92.852214462957591</v>
+        <v>81.42265735554912</v>
       </c>
       <c r="D222" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="3">
+      <c r="A223" s="13">
         <v>3412.5310679611648</v>
       </c>
       <c r="B223" s="4">
         <v>76.149823874910538</v>
       </c>
       <c r="C223" s="4">
-        <v>94.508072116326488</v>
+        <v>83.409686539591775</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="3">
+      <c r="A224" s="13">
         <v>3413.0694174757277</v>
       </c>
       <c r="B224" s="4">
         <v>81.092597655791167</v>
       </c>
       <c r="C224" s="4">
-        <v>95.529184335903977</v>
+        <v>84.635021203084762</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="3">
+      <c r="A225" s="13">
         <v>3413.6077669902907</v>
       </c>
       <c r="B225" s="4">
         <v>85.100252072721446</v>
       </c>
       <c r="C225" s="4">
-        <v>96.357113162588433</v>
+        <v>85.628535795106117</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="3">
+      <c r="A226" s="13">
         <v>3414.146116504854</v>
       </c>
       <c r="B226" s="4">
         <v>94.31786391108507</v>
       </c>
       <c r="C226" s="4">
-        <v>98.261350843844042</v>
+        <v>87.91362101261285</v>
       </c>
       <c r="D226" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="3">
+      <c r="A227" s="13">
         <v>3414.684466019417</v>
       </c>
       <c r="B227" s="4">
         <v>79.689938648137669</v>
       </c>
       <c r="C227" s="4">
-        <v>95.239413386208554</v>
+        <v>84.28729606345027</v>
       </c>
       <c r="D227" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="3">
+      <c r="A228" s="13">
         <v>3415.2228155339803</v>
       </c>
       <c r="B228" s="4">
         <v>80.491462852099701</v>
       </c>
       <c r="C228" s="4">
-        <v>95.404997771664057</v>
+        <v>84.485997325996863</v>
       </c>
       <c r="D228" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="3">
+      <c r="A229" s="13">
         <v>3415.7611650485433</v>
       </c>
       <c r="B229" s="4">
         <v>73.745251263024457</v>
       </c>
       <c r="C229" s="4">
-        <v>94.011318959959951</v>
+        <v>82.813582751951941</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="3">
+      <c r="A230" s="13">
         <v>3416.2995145631062</v>
       </c>
       <c r="B230" s="4">
         <v>70.271937409503522</v>
       </c>
       <c r="C230" s="4">
-        <v>93.293777883737334</v>
+        <v>81.952533460484801</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="3">
+      <c r="A231" s="13">
         <v>3416.8378640776696</v>
       </c>
       <c r="B231" s="4">
         <v>70.806284652336856</v>
       </c>
       <c r="C231" s="4">
-        <v>93.404167014080556</v>
+        <v>82.085000416896662</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="3">
+      <c r="A232" s="13">
         <v>3417.3762135922325</v>
       </c>
       <c r="B232" s="4">
         <v>78.821593486197372</v>
       </c>
       <c r="C232" s="4">
-        <v>95.060024667449454</v>
+        <v>84.072029600939345</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="3">
+      <c r="A233" s="13">
         <v>3417.9145631067959</v>
       </c>
       <c r="B233" s="4">
         <v>84.499103910181901</v>
       </c>
       <c r="C233" s="4">
-        <v>96.232923838585748</v>
+        <v>85.479508606302915</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="3">
+      <c r="A234" s="13">
         <v>3418.4529126213588</v>
       </c>
       <c r="B234" s="4">
         <v>80.291066772405117</v>
       </c>
       <c r="C234" s="4">
-        <v>95.363598570567092</v>
+        <v>84.436318284680496</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="3">
+      <c r="A235" s="13">
         <v>3418.9912621359217</v>
       </c>
       <c r="B235" s="4">
         <v>82.762453662845445</v>
       </c>
       <c r="C235" s="4">
-        <v>95.874154680355829</v>
+        <v>85.04898561642699</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="3">
+      <c r="A236" s="13">
         <v>3419.5296116504851</v>
       </c>
       <c r="B236" s="4">
         <v>84.833075111592763</v>
       </c>
       <c r="C236" s="4">
-        <v>96.301917907476138</v>
+        <v>85.562301488971357</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="3">
+      <c r="A237" s="13">
         <v>3420.067961165048</v>
       </c>
       <c r="B237" s="4">
         <v>87.772021684008294</v>
       </c>
       <c r="C237" s="4">
-        <v>96.909065713711385</v>
+        <v>86.290878856453674</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="3">
+      <c r="A238" s="13">
         <v>3420.6063106796114</v>
       </c>
       <c r="B238" s="4">
         <v>76.817772957156279</v>
       </c>
       <c r="C238" s="4">
-        <v>94.646061633988609</v>
+        <v>83.575273960786319</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="3">
+      <c r="A239" s="13">
         <v>3421.1446601941743</v>
       </c>
       <c r="B239" s="4">
         <v>53.172625256115815</v>
       </c>
       <c r="C239" s="4">
-        <v>89.761284316313109</v>
+        <v>77.713541179575742</v>
       </c>
       <c r="D239" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="3">
+      <c r="A240" s="13">
         <v>3421.6830097087377</v>
       </c>
       <c r="B240" s="4">
         <v>41.149655325901008</v>
       </c>
       <c r="C240" s="4">
-        <v>87.277496456378373</v>
+        <v>74.732995747654059</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="3">
+      <c r="A241" s="13">
         <v>3422.2213592233006</v>
       </c>
       <c r="B241" s="4">
         <v>48.096269674094842</v>
       </c>
       <c r="C241" s="4">
-        <v>88.712575849060855</v>
+        <v>76.45509101887302</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="3">
+      <c r="A242" s="13">
         <v>3422.7597087378635</v>
       </c>
       <c r="B242" s="4">
         <v>47.5619224312615</v>
       </c>
       <c r="C242" s="4">
-        <v>88.602186718717633</v>
+        <v>76.322624062461159</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="3">
+      <c r="A243" s="13">
         <v>3423.2980582524269</v>
       </c>
       <c r="B243" s="4">
         <v>43.487467094625039</v>
       </c>
       <c r="C243" s="4">
-        <v>87.760457698373727</v>
+        <v>75.312549238048462</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="3">
+      <c r="A244" s="13">
         <v>3423.8364077669899</v>
       </c>
       <c r="B244" s="4">
         <v>57.313854794762335</v>
       </c>
       <c r="C244" s="4">
-        <v>90.616808010790947</v>
+        <v>78.740169612949131</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="3">
+      <c r="A245" s="13">
         <v>3424.3747572815532</v>
       </c>
       <c r="B245" s="4">
         <v>63.726101861850751</v>
       </c>
       <c r="C245" s="4">
-        <v>91.94149413348606</v>
+        <v>80.329792960183283</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="3">
+      <c r="A246" s="13">
         <v>3424.9131067961162</v>
       </c>
       <c r="B246" s="4">
         <v>57.781434515009622</v>
       </c>
       <c r="C246" s="4">
-        <v>90.71340384688159</v>
+        <v>78.856084616257917</v>
       </c>
       <c r="D246" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="3">
+      <c r="A247" s="13">
         <v>3425.4514563106791</v>
       </c>
       <c r="B247" s="4">
         <v>48.630623596352216</v>
       </c>
       <c r="C247" s="4">
-        <v>88.822966359285445</v>
+        <v>76.58755963114254</v>
       </c>
       <c r="D247" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="3">
+      <c r="A248" s="13">
         <v>3425.9898058252425</v>
       </c>
       <c r="B248" s="4">
         <v>36.474058506149056</v>
       </c>
       <c r="C248" s="4">
-        <v>86.311579491913193</v>
+        <v>73.573895390295831</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="3">
+      <c r="A249" s="13">
         <v>3426.5281553398054</v>
       </c>
       <c r="B249" s="4">
         <v>34.603826457672298</v>
       </c>
       <c r="C249" s="4">
-        <v>85.925214086008495</v>
+        <v>73.1102569032102</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="3">
+      <c r="A250" s="13">
         <v>3427.0665048543688</v>
       </c>
       <c r="B250" s="4">
         <v>46.760364830179348</v>
       </c>
       <c r="C250" s="4">
-        <v>88.436595433855246</v>
+        <v>76.123914520626272</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="3">
+      <c r="A251" s="13">
         <v>3427.6048543689317</v>
       </c>
       <c r="B251" s="4">
         <v>46.426386949344462</v>
       </c>
       <c r="C251" s="4">
-        <v>88.367599985083487</v>
+        <v>76.041119982100184</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="3">
+      <c r="A252" s="13">
         <v>3428.1432038834946</v>
       </c>
       <c r="B252" s="4">
         <v>32.867156172063758</v>
       </c>
       <c r="C252" s="4">
-        <v>85.566440788134429</v>
+        <v>72.679728945761312</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="3">
+      <c r="A253" s="13">
         <v>3428.681553398058</v>
       </c>
       <c r="B253" s="4">
         <v>26.788880306386197</v>
       </c>
       <c r="C253" s="4">
-        <v>84.310748734329678</v>
+        <v>71.172898481195617</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="3">
+      <c r="A254" s="13">
         <v>3429.2199029126209</v>
       </c>
       <c r="B254" s="4">
         <v>24.117110695099363</v>
       </c>
       <c r="C254" s="4">
-        <v>83.758796183206712</v>
+        <v>70.51055541984806</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="3">
+      <c r="A255" s="13">
         <v>3429.7582524271843</v>
       </c>
       <c r="B255" s="4">
         <v>37.542752991815732</v>
       </c>
       <c r="C255" s="4">
-        <v>86.532357752599623</v>
+        <v>73.838829303119553</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="3">
+      <c r="A256" s="13">
         <v>3430.2966019417472</v>
       </c>
       <c r="B256" s="4">
         <v>57.914996277877869</v>
       </c>
       <c r="C256" s="4">
-        <v>90.740995954912236</v>
+        <v>78.889195145894689</v>
       </c>
       <c r="D256" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="3">
+      <c r="A257" s="13">
         <v>3430.8349514563101</v>
       </c>
       <c r="B257" s="4">
         <v>55.577204547425914</v>
       </c>
       <c r="C257" s="4">
-        <v>90.258038852561015</v>
+        <v>78.30964662307322</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A258" s="3">
+      <c r="A258" s="13">
         <v>3431.3733009708735</v>
       </c>
       <c r="B258" s="4">
         <v>44.288991298587078</v>
       </c>
       <c r="C258" s="4">
-        <v>87.92604208382923</v>
+        <v>75.511250500595082</v>
       </c>
       <c r="D258" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A259" s="3">
+      <c r="A259" s="13">
         <v>3431.9116504854364</v>
       </c>
       <c r="B259" s="4">
         <v>42.819511332955287</v>
       </c>
       <c r="C259" s="4">
-        <v>87.622466800830239</v>
+        <v>75.146960160996287</v>
       </c>
       <c r="D259" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A260" s="3">
+      <c r="A260" s="13">
         <v>3432.45</v>
       </c>
       <c r="B260" s="4">
         <v>42.552341051250629</v>
       </c>
       <c r="C260" s="4">
-        <v>87.567272925599326</v>
+        <v>75.080727510719186</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A261" s="3">
+      <c r="A261" s="13">
         <v>3432.9883495145627</v>
       </c>
       <c r="B261" s="4">
         <v>47.02754847073205</v>
       </c>
       <c r="C261" s="4">
-        <v>88.491792068848909</v>
+        <v>76.190150482618691</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A262" s="3">
+      <c r="A262" s="13">
         <v>3433.5266990291257</v>
       </c>
       <c r="B262" s="4">
         <v>35.271768860493992</v>
       </c>
       <c r="C262" s="4">
-        <v>86.063202223789233</v>
+        <v>73.275842668547071</v>
       </c>
       <c r="D262" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A263" s="3">
+      <c r="A263" s="13">
         <v>3434.065048543689</v>
       </c>
       <c r="B263" s="4">
         <v>41.884385289580869</v>
       </c>
       <c r="C263" s="4">
-        <v>87.429282028055823</v>
+        <v>74.915138433666982</v>
       </c>
       <c r="D263" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="3">
+      <c r="A264" s="13">
         <v>3434.603398058252</v>
       </c>
       <c r="B264" s="4">
         <v>48.163037196680918</v>
       </c>
       <c r="C264" s="4">
-        <v>88.72636914331342</v>
+        <v>76.471642971976109</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="3">
+      <c r="A265" s="13">
         <v>3435.1417475728153</v>
       </c>
       <c r="B265" s="4">
         <v>35.739308504197119</v>
       </c>
       <c r="C265" s="4">
-        <v>86.159789780591623</v>
+        <v>73.391747736709931</v>
       </c>
       <c r="D265" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A266" s="3">
+      <c r="A266" s="13">
         <v>3435.6800970873783</v>
       </c>
       <c r="B266" s="4">
         <v>33.468311014027329</v>
       </c>
       <c r="C266" s="4">
-        <v>85.690631492018468</v>
+        <v>72.828757790422173</v>
       </c>
       <c r="D266" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="3">
+      <c r="A267" s="13">
         <v>3436.2184466019412</v>
       </c>
       <c r="B267" s="4">
         <v>49.632530521160746</v>
       </c>
       <c r="C267" s="4">
-        <v>89.029947186075162</v>
+        <v>76.835936623290195</v>
       </c>
       <c r="D267" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A268" s="3">
+      <c r="A268" s="13">
         <v>3436.7567961165046</v>
       </c>
       <c r="B268" s="4">
         <v>70.138348928939166</v>
       </c>
       <c r="C268" s="4">
-        <v>93.266180256181201</v>
+        <v>81.919416307417421</v>
       </c>
       <c r="D268" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" s="3">
+      <c r="A269" s="13">
         <v>3437.2951456310675</v>
       </c>
       <c r="B269" s="4">
         <v>71.140255853747689</v>
       </c>
       <c r="C269" s="4">
-        <v>93.473161082970933</v>
+        <v>82.167793299565119</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A270" s="3">
+      <c r="A270" s="13">
         <v>3437.8334951456309</v>
       </c>
       <c r="B270" s="4">
         <v>58.382555959853065</v>
       </c>
       <c r="C270" s="4">
-        <v>90.837587651358746</v>
+        <v>79.005105181630512</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="3">
+      <c r="A271" s="13">
         <v>3438.3718446601938</v>
       </c>
       <c r="B271" s="4">
         <v>49.766098963453004</v>
       </c>
       <c r="C271" s="4">
-        <v>89.057540673987191</v>
+        <v>76.86904880878464</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A272" s="3">
+      <c r="A272" s="13">
         <v>3438.9101941747567</v>
       </c>
       <c r="B272" s="4">
         <v>33.267928293180809</v>
       </c>
       <c r="C272" s="4">
-        <v>85.64923505068424</v>
+        <v>72.779082060821096</v>
       </c>
       <c r="D272" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" s="3">
+      <c r="A273" s="13">
         <v>3439.4485436893201</v>
       </c>
       <c r="B273" s="4">
         <v>27.189665786351316</v>
       </c>
       <c r="C273" s="4">
-        <v>84.393545756642254</v>
+        <v>71.272254907970705</v>
       </c>
       <c r="D273" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="3">
+      <c r="A274" s="13">
         <v>3439.986893203883</v>
       </c>
       <c r="B274" s="4">
         <v>40.8824716853483</v>
       </c>
       <c r="C274" s="4">
-        <v>87.222299821384709</v>
+        <v>74.66675978566164</v>
       </c>
       <c r="D274" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A275" s="3">
+      <c r="A275" s="13">
         <v>3440.5252427184464</v>
       </c>
       <c r="B275" s="4">
         <v>54.040930341511945</v>
       </c>
       <c r="C275" s="4">
-        <v>89.940664755783928</v>
+        <v>77.928797706940728</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A276" s="3">
+      <c r="A276" s="13">
         <v>3441.0635922330093</v>
       </c>
       <c r="B276" s="4">
         <v>62.523798857347664</v>
       </c>
       <c r="C276" s="4">
-        <v>91.693114105599363</v>
+        <v>80.031736926719219</v>
       </c>
       <c r="D276" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A277" s="3">
+      <c r="A277" s="13">
         <v>3441.6019417475723</v>
       </c>
       <c r="B277" s="4">
         <v>66.264276313149239</v>
       </c>
       <c r="C277" s="4">
-        <v>92.465847677171524</v>
+        <v>80.959017212605815</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A278" s="3">
+      <c r="A278" s="13">
         <v>3442.1402912621356</v>
       </c>
       <c r="B278" s="4">
         <v>72.676530059661673</v>
       </c>
       <c r="C278" s="4">
-        <v>93.790535179748005</v>
+        <v>82.548642215697612</v>
       </c>
       <c r="D278" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" s="3">
+      <c r="A279" s="13">
         <v>3442.6786407766986</v>
       </c>
       <c r="B279" s="4">
         <v>67.600181157064711</v>
       </c>
       <c r="C279" s="4">
-        <v>92.741828092377119</v>
+        <v>81.290193710852549</v>
       </c>
       <c r="D279" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A280" s="3">
+      <c r="A280" s="13">
         <v>3443.2169902912619</v>
       </c>
       <c r="B280" s="4">
         <v>63.859690342415092</v>
       </c>
       <c r="C280" s="4">
-        <v>91.969091761042222</v>
+        <v>80.362910113250649</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="3">
+      <c r="A281" s="13">
         <v>3443.7553398058249</v>
       </c>
       <c r="B281" s="4">
         <v>74.413173627574096</v>
       </c>
       <c r="C281" s="4">
-        <v>94.14930295809657</v>
+        <v>82.979163549715878</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A282" s="3">
+      <c r="A282" s="13">
         <v>3444.2936893203878</v>
       </c>
       <c r="B282" s="4">
         <v>65.930305111738377</v>
       </c>
       <c r="C282" s="4">
-        <v>92.396853608281148</v>
+        <v>80.876224329937372</v>
       </c>
       <c r="D282" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" s="3">
+      <c r="A283" s="13">
         <v>3444.8320388349512</v>
       </c>
       <c r="B283" s="4">
         <v>64.460831825530619</v>
       </c>
       <c r="C283" s="4">
-        <v>92.093279705163496</v>
+        <v>80.511935646196207</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A284" s="3">
+      <c r="A284" s="13">
         <v>3445.3703883495141</v>
       </c>
       <c r="B284" s="4">
         <v>64.460831825530619</v>
       </c>
       <c r="C284" s="4">
-        <v>92.093279705163496</v>
+        <v>80.511935646196207</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A285" s="3">
+      <c r="A285" s="13">
         <v>3445.9087378640775</v>
       </c>
       <c r="B285" s="4">
         <v>64.527626065812768</v>
       </c>
       <c r="C285" s="4">
-        <v>92.107078518941577</v>
+        <v>80.528494222729904</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A286" s="3">
+      <c r="A286" s="13">
         <v>3446.4470873786404</v>
       </c>
       <c r="B286" s="4">
         <v>70.605908610914355</v>
       </c>
       <c r="C286" s="4">
-        <v>93.362771952627696</v>
+        <v>82.035326343153244</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A287" s="3">
+      <c r="A287" s="13">
         <v>3446.9854368932033</v>
       </c>
       <c r="B287" s="4">
         <v>68.201335999028302</v>
       </c>
       <c r="C287" s="4">
-        <v>92.866018796261173</v>
+        <v>81.439222555513396</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A288" s="3">
+      <c r="A288" s="13">
         <v>3447.5237864077667</v>
       </c>
       <c r="B288" s="4">
         <v>66.932245433667035</v>
       </c>
       <c r="C288" s="4">
-        <v>92.60384133447775</v>
+        <v>81.124609601373322</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A289" s="3">
+      <c r="A289" s="13">
         <v>3448.0621359223296</v>
       </c>
       <c r="B289" s="4">
         <v>63.525719141004252</v>
       </c>
       <c r="C289" s="4">
-        <v>91.900097692151846</v>
+        <v>80.280117230582221</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A290" s="3">
+      <c r="A290" s="13">
         <v>3448.600485436893</v>
       </c>
       <c r="B290" s="4">
         <v>61.121119811422069</v>
       </c>
       <c r="C290" s="4">
-        <v>91.403339016259793</v>
+        <v>79.684006819511751</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A291" s="3">
+      <c r="A291" s="13">
         <v>3449.1388349514559</v>
       </c>
       <c r="B291" s="4">
         <v>66.063893592302719</v>
       </c>
       <c r="C291" s="4">
-        <v>92.424451235837296</v>
+        <v>80.909341483004738</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A292" s="3">
+      <c r="A292" s="13">
         <v>3449.6771844660188</v>
       </c>
       <c r="B292" s="4">
         <v>75.28149875124231</v>
       </c>
       <c r="C292" s="4">
-        <v>94.328687537211522</v>
+        <v>83.194425044653826</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A293" s="3">
+      <c r="A293" s="13">
         <v>3450.2155339805822</v>
       </c>
       <c r="B293" s="4">
         <v>73.878819705316729</v>
       </c>
       <c r="C293" s="4">
-        <v>94.038912447871965</v>
+        <v>82.846694937446358</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A294" s="3">
+      <c r="A294" s="13">
         <v>3450.7538834951451</v>
       </c>
       <c r="B294" s="4">
         <v>55.911169069412743</v>
       </c>
       <c r="C294" s="4">
-        <v>90.327031541570022</v>
+        <v>78.392437849884033</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A295" s="3">
+      <c r="A295" s="13">
         <v>3451.2922330097085</v>
       </c>
       <c r="B295" s="4">
         <v>44.95691366313671</v>
       </c>
       <c r="C295" s="4">
-        <v>88.064026081965864</v>
+        <v>75.676831298359019</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A296" s="3">
+      <c r="A296" s="13">
         <v>3451.8305825242714</v>
       </c>
       <c r="B296" s="4">
         <v>46.626776349615007</v>
       </c>
       <c r="C296" s="4">
-        <v>88.408997806299084</v>
+        <v>76.090797367558906</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A297" s="3">
+      <c r="A297" s="13">
         <v>3452.3689320388344</v>
       </c>
       <c r="B297" s="4">
         <v>55.644018825980154</v>
       </c>
       <c r="C297" s="4">
-        <v>90.271841805983229</v>
+        <v>78.32621016717988</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A298" s="3">
+      <c r="A298" s="13">
         <v>3452.9072815533978</v>
       </c>
       <c r="B298" s="4">
         <v>57.313874833034426</v>
       </c>
       <c r="C298" s="4">
-        <v>90.616812150435081</v>
+        <v>78.740174580522094</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A299" s="3">
+      <c r="A299" s="13">
         <v>3453.4456310679607</v>
       </c>
       <c r="B299" s="4">
         <v>46.827165749885538</v>
       </c>
       <c r="C299" s="4">
-        <v>88.450395627514681</v>
+        <v>76.140474753017614</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A300" s="3">
+      <c r="A300" s="13">
         <v>3453.9839805825241</v>
       </c>
       <c r="B300" s="4">
         <v>24.785073136193159</v>
       </c>
       <c r="C300" s="4">
-        <v>83.896788460631598</v>
+        <v>70.676146152757894</v>
       </c>
       <c r="D300" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A301" s="3">
+      <c r="A301" s="13">
         <v>3454.522330097087</v>
       </c>
       <c r="B301" s="4">
         <v>23.582770131690058</v>
       </c>
       <c r="C301" s="4">
-        <v>83.648408432744873</v>
+        <v>70.378090119293859</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A302" s="3">
+      <c r="A302" s="13">
         <v>3455.0606796116499</v>
       </c>
       <c r="B302" s="4">
         <v>46.893973349015774</v>
       </c>
       <c r="C302" s="4">
-        <v>88.464197201055526</v>
+        <v>76.157036641266615</v>
       </c>
       <c r="D302" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A303" s="3">
+      <c r="A303" s="13">
         <v>3455.5990291262133</v>
       </c>
       <c r="B303" s="4">
         <v>59.65167324291042</v>
       </c>
       <c r="C303" s="4">
-        <v>91.099770632667685</v>
+        <v>79.319724759201222</v>
       </c>
       <c r="D303" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A304" s="3">
+      <c r="A304" s="13">
         <v>3456.1373786407762</v>
       </c>
       <c r="B304" s="4">
         <v>60.119219566037565</v>
       </c>
       <c r="C304" s="4">
-        <v>91.196359569351443</v>
+        <v>79.435631483221727</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A305" s="3">
+      <c r="A305" s="13">
         <v>3456.6757281553396</v>
       </c>
       <c r="B305" s="4">
         <v>42.752730451521167</v>
       </c>
       <c r="C305" s="4">
-        <v>87.608670746814909</v>
+        <v>75.130404896177893</v>
       </c>
       <c r="D305" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A306" s="3">
+      <c r="A306" s="13">
         <v>3457.2140776699025</v>
       </c>
       <c r="B306" s="4">
         <v>37.876750910922695</v>
       </c>
       <c r="C306" s="4">
-        <v>86.6013573410155</v>
+        <v>73.921628809218603</v>
       </c>
       <c r="D306" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A307" s="3">
+      <c r="A307" s="13">
         <v>3457.7524271844659</v>
       </c>
       <c r="B307" s="4">
         <v>36.340463346160682</v>
       </c>
       <c r="C307" s="4">
-        <v>86.283980484475663</v>
+        <v>73.540776581370793</v>
       </c>
       <c r="D307" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A308" s="3">
+      <c r="A308" s="13">
         <v>3458.2907766990288</v>
       </c>
       <c r="B308" s="4">
         <v>36.60763362786534</v>
       </c>
       <c r="C308" s="4">
-        <v>86.33917435970659</v>
+        <v>73.607009231647908</v>
       </c>
       <c r="D308" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A309" s="3">
+      <c r="A309" s="13">
         <v>3458.8291262135917</v>
       </c>
       <c r="B309" s="4">
         <v>42.819504653531261</v>
       </c>
       <c r="C309" s="4">
-        <v>87.622465420948856</v>
+        <v>75.146958505138628</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A310" s="3">
+      <c r="A310" s="13">
         <v>3459.3674757281551</v>
       </c>
       <c r="B310" s="4">
         <v>40.481726281927358</v>
       </c>
       <c r="C310" s="4">
-        <v>87.139511078360385</v>
+        <v>74.567413294032463</v>
       </c>
       <c r="D310" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A311" s="3">
+      <c r="A311" s="13">
         <v>3459.905825242718</v>
       </c>
       <c r="B311" s="4">
         <v>40.615314762491707</v>
       </c>
       <c r="C311" s="4">
-        <v>87.167108705916547</v>
+        <v>74.600530447099857</v>
       </c>
       <c r="D311" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A312" s="3">
+      <c r="A312" s="13">
         <v>3460.4441747572814</v>
       </c>
       <c r="B312" s="4">
         <v>41.216449566183186</v>
       </c>
       <c r="C312" s="4">
-        <v>87.291295270156468</v>
+        <v>74.749554324187756</v>
       </c>
       <c r="D312" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A313" s="3">
+      <c r="A313" s="13">
         <v>3460.9825242718443</v>
       </c>
       <c r="B313" s="4">
         <v>44.689756740280103</v>
       </c>
       <c r="C313" s="4">
-        <v>88.008834966497687</v>
+        <v>75.610601959797236</v>
       </c>
       <c r="D313" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A314" s="3">
+      <c r="A314" s="13">
         <v>3461.5208737864073</v>
       </c>
       <c r="B314" s="4">
         <v>49.432141120890215</v>
       </c>
       <c r="C314" s="4">
-        <v>88.98854936485958</v>
+        <v>76.786259237831487</v>
       </c>
       <c r="D314" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A315" s="3">
+      <c r="A315" s="13">
         <v>3462.0592233009706</v>
       </c>
       <c r="B315" s="4">
         <v>53.439808896668524</v>
       </c>
       <c r="C315" s="4">
-        <v>89.816480951306787</v>
+        <v>77.779777141568132</v>
       </c>
       <c r="D315" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A316" s="3">
+      <c r="A316" s="13">
         <v>3462.5975728155336</v>
       </c>
       <c r="B316" s="4">
         <v>60.787175327707317</v>
       </c>
       <c r="C316" s="4">
-        <v>91.334350466894932</v>
+        <v>79.60122056027393</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A317" s="3">
+      <c r="A317" s="13">
         <v>3463.1359223300969</v>
       </c>
       <c r="B317" s="4">
         <v>69.603995006681799</v>
       </c>
       <c r="C317" s="4">
-        <v>93.155789745956582</v>
+        <v>81.786947695147916</v>
       </c>
       <c r="D317" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A318" s="3">
+      <c r="A318" s="13">
         <v>3463.6742718446599</v>
       </c>
       <c r="B318" s="4">
         <v>63.99327214355543</v>
       </c>
       <c r="C318" s="4">
-        <v>91.996688008716987</v>
+        <v>80.396025610460384</v>
       </c>
       <c r="D318" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A319" s="3">
+      <c r="A319" s="13">
         <v>3464.2126213592228</v>
       </c>
       <c r="B319" s="4">
         <v>58.582938680699577</v>
       </c>
       <c r="C319" s="4">
-        <v>90.878984092692974</v>
+        <v>79.054780911231575</v>
       </c>
       <c r="D319" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A320" s="3">
+      <c r="A320" s="13">
         <v>3464.7509708737862</v>
       </c>
       <c r="B320" s="4">
         <v>63.792889422708903</v>
       </c>
       <c r="C320" s="4">
-        <v>91.955291567382773</v>
+        <v>80.346349880859322</v>
       </c>
       <c r="D320" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A321" s="3">
+      <c r="A321" s="13">
         <v>3465.2893203883491</v>
       </c>
       <c r="B321" s="4">
         <v>62.323422815925163</v>
       </c>
       <c r="C321" s="4">
-        <v>91.651719044146517</v>
+        <v>79.982062852975815</v>
       </c>
       <c r="D321" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A322" s="3">
+      <c r="A322" s="13">
         <v>3465.8276699029125</v>
       </c>
       <c r="B322" s="4">
         <v>54.642105221747599</v>
       </c>
       <c r="C322" s="4">
-        <v>90.064859599312115</v>
+        <v>78.077831519174538</v>
       </c>
       <c r="D322" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A323" s="3">
+      <c r="A323" s="13">
         <v>3466.3660194174754</v>
       </c>
       <c r="B323" s="4">
         <v>46.426420346464603</v>
       </c>
       <c r="C323" s="4">
-        <v>88.367606884490371</v>
+        <v>76.041128261388451</v>
       </c>
       <c r="D323" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A324" s="3">
+      <c r="A324" s="13">
         <v>3466.9043689320383</v>
       </c>
       <c r="B324" s="4">
         <v>51.569570168767733</v>
       </c>
       <c r="C324" s="4">
-        <v>89.430114165520706</v>
+        <v>77.316136998624842</v>
       </c>
       <c r="D324" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A325" s="3">
+      <c r="A325" s="13">
         <v>3467.4427184466017</v>
       </c>
       <c r="B325" s="4">
         <v>51.970322251612707</v>
       </c>
       <c r="C325" s="4">
-        <v>89.512904288426398</v>
+        <v>77.415485146111678</v>
       </c>
       <c r="D325" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A326" s="3">
+      <c r="A326" s="13">
         <v>3467.9810679611646</v>
       </c>
       <c r="B326" s="4">
         <v>62.857790097030602</v>
       </c>
       <c r="C326" s="4">
-        <v>91.762112314133873</v>
+        <v>80.114534776960639</v>
       </c>
       <c r="D326" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A327" s="3">
+      <c r="A327" s="13">
         <v>3468.519417475728</v>
       </c>
       <c r="B327" s="4">
         <v>68.134528399898073</v>
       </c>
       <c r="C327" s="4">
-        <v>92.852217222720341</v>
+        <v>81.42266066726441</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A328" s="3">
+      <c r="A328" s="13">
         <v>3469.0577669902909</v>
       </c>
       <c r="B328" s="4">
         <v>52.371101052153769</v>
       </c>
       <c r="C328" s="4">
-        <v>89.595699930857592</v>
+        <v>77.514839917029107</v>
       </c>
       <c r="D328" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A329" s="3">
+      <c r="A329" s="13">
         <v>3469.5961165048539</v>
       </c>
       <c r="B329" s="4">
         <v>66.130714550280999</v>
       </c>
       <c r="C329" s="4">
-        <v>92.438255569140864</v>
+        <v>80.925906682969043</v>
       </c>
       <c r="D329" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A330" s="3">
+      <c r="A330" s="13">
         <v>3470.1344660194172</v>
       </c>
       <c r="B330" s="4">
         <v>68.000939919333732</v>
       </c>
       <c r="C330" s="4">
-        <v>92.824619595164194</v>
+        <v>81.389543514197044</v>
       </c>
       <c r="D330" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A331" s="3">
+      <c r="A331" s="13">
         <v>3470.6728155339802</v>
       </c>
       <c r="B331" s="4">
         <v>72.676543418509709</v>
       </c>
       <c r="C331" s="4">
-        <v>93.790537939510756</v>
+        <v>82.548645527412916</v>
       </c>
       <c r="D331" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A332" s="3">
+      <c r="A332" s="13">
         <v>3471.2111650485435</v>
       </c>
       <c r="B332" s="4">
         <v>66.731842674548446</v>
       </c>
       <c r="C332" s="4">
-        <v>92.562440753499402</v>
+        <v>81.074928904199282</v>
       </c>
       <c r="D332" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A333" s="3">
+      <c r="A333" s="13">
         <v>3471.7495145631065</v>
       </c>
       <c r="B333" s="4">
         <v>57.647825996173196</v>
       </c>
       <c r="C333" s="4">
-        <v>90.685802079681309</v>
+        <v>78.822962495617588</v>
       </c>
       <c r="D333" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A334" s="3">
+      <c r="A334" s="13">
         <v>3472.2878640776694</v>
       </c>
       <c r="B334" s="4">
         <v>57.781427835585603</v>
       </c>
       <c r="C334" s="4">
-        <v>90.713402467000222</v>
+        <v>78.856082960400272</v>
       </c>
       <c r="D334" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A335" s="3">
+      <c r="A335" s="13">
         <v>3472.8262135922328</v>
       </c>
       <c r="B335" s="4">
         <v>64.928404866353873</v>
       </c>
       <c r="C335" s="4">
-        <v>92.189874161372785</v>
+        <v>80.627848993647333</v>
       </c>
       <c r="D335" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A336" s="3">
+      <c r="A336" s="13">
         <v>3473.3645631067957</v>
       </c>
       <c r="B336" s="4">
         <v>67.800570557335277</v>
       </c>
       <c r="C336" s="4">
-        <v>92.78322591359273</v>
+        <v>81.339871096311271</v>
       </c>
       <c r="D336" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A337" s="3">
+      <c r="A337" s="13">
         <v>3473.9029126213591</v>
       </c>
       <c r="B337" s="4">
         <v>62.056272572492595</v>
       </c>
       <c r="C337" s="4">
-        <v>91.596529308559724</v>
+        <v>79.915835170271663</v>
       </c>
       <c r="D337" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A338" s="3">
+      <c r="A338" s="13">
         <v>3474.441262135922</v>
       </c>
       <c r="B338" s="4">
         <v>62.390237094479424</v>
       </c>
       <c r="C338" s="4">
-        <v>91.665521997568732</v>
+        <v>79.998626397082461</v>
       </c>
       <c r="D338" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" s="3">
+      <c r="A339" s="13">
         <v>3474.9796116504849</v>
       </c>
       <c r="B339" s="4">
         <v>70.539114370632191</v>
       </c>
       <c r="C339" s="4">
-        <v>93.34897313884963</v>
+        <v>82.018767766619561</v>
       </c>
       <c r="D339" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A340" s="3">
+      <c r="A340" s="13">
         <v>3475.5179611650483</v>
       </c>
       <c r="B340" s="4">
         <v>71.741404016287248</v>
       </c>
       <c r="C340" s="4">
-        <v>93.59735040697359</v>
+        <v>82.316820488368307</v>
       </c>
       <c r="D340" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A341" s="3">
+      <c r="A341" s="13">
         <v>3476.0563106796112</v>
       </c>
       <c r="B341" s="4">
         <v>79.355954087878757</v>
       </c>
       <c r="C341" s="4">
-        <v>95.170416557555427</v>
+        <v>84.20449986906651</v>
       </c>
       <c r="D341" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A342" s="3">
+      <c r="A342" s="13">
         <v>3476.5946601941746</v>
       </c>
       <c r="B342" s="4">
         <v>82.428502499706667</v>
       </c>
       <c r="C342" s="4">
-        <v>95.805164751109587</v>
+        <v>84.96619770133151</v>
       </c>
       <c r="D342" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A343" s="3">
+      <c r="A343" s="13">
         <v>3477.1330097087375</v>
       </c>
       <c r="B343" s="4">
         <v>83.163232463386521</v>
       </c>
       <c r="C343" s="4">
-        <v>95.956950322787023</v>
+        <v>85.148340387344433</v>
       </c>
       <c r="D343" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A344" s="3">
+      <c r="A344" s="13">
         <v>3477.6713592233004</v>
       </c>
       <c r="B344" s="4">
         <v>69.336831404401181</v>
       </c>
       <c r="C344" s="4">
-        <v>93.100597250607052</v>
+        <v>81.720716700728474</v>
       </c>
       <c r="D344" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A345" s="3">
+      <c r="A345" s="13">
         <v>3478.2097087378638</v>
       </c>
       <c r="B345" s="4">
         <v>71.874992496851604</v>
       </c>
       <c r="C345" s="4">
-        <v>93.624948034529751</v>
+        <v>82.349937641435687</v>
       </c>
       <c r="D345" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A346" s="3">
+      <c r="A346" s="13">
         <v>3478.7480582524267</v>
       </c>
       <c r="B346" s="4">
         <v>76.550562598907462</v>
       </c>
       <c r="C346" s="4">
-        <v>94.59085947946943</v>
+        <v>83.509031375363307</v>
       </c>
       <c r="D346" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A347" s="3">
+      <c r="A347" s="13">
         <v>3479.2864077669901</v>
       </c>
       <c r="B347" s="4">
         <v>70.071521291536868</v>
       </c>
       <c r="C347" s="4">
-        <v>93.252374542996222</v>
+        <v>81.902849451595472</v>
       </c>
       <c r="D347" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A348" s="3">
+      <c r="A348" s="13">
         <v>3479.824757281553</v>
       </c>
       <c r="B348" s="4">
         <v>59.117285923532904</v>
       </c>
       <c r="C348" s="4">
-        <v>90.989373223036196</v>
+        <v>79.187247867643435</v>
       </c>
       <c r="D348" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A349" s="3">
+      <c r="A349" s="13">
         <v>3480.363106796116</v>
       </c>
       <c r="B349" s="4">
         <v>66.598247514560086</v>
       </c>
       <c r="C349" s="4">
-        <v>92.534841746061886</v>
+        <v>81.041810095274258</v>
       </c>
       <c r="D349" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A350" s="3">
+      <c r="A350" s="13">
         <v>3480.9014563106794</v>
       </c>
       <c r="B350" s="4">
         <v>68.401685322754673</v>
       </c>
       <c r="C350" s="4">
-        <v>92.907408338188503</v>
+        <v>81.488890005826207</v>
       </c>
       <c r="D350" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A351" s="3">
+      <c r="A351" s="13">
         <v>3481.4398058252423</v>
       </c>
       <c r="B351" s="4">
         <v>74.212770868455493</v>
       </c>
       <c r="C351" s="4">
-        <v>94.107902377118208</v>
+        <v>82.929482852541838</v>
       </c>
       <c r="D351" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A352" s="3">
+      <c r="A352" s="13">
         <v>3481.9781553398057</v>
       </c>
       <c r="B352" s="4">
         <v>71.74139733686323</v>
       </c>
       <c r="C352" s="4">
-        <v>93.597349027092207</v>
+        <v>82.316818832510663</v>
       </c>
       <c r="D352" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A353" s="3">
+      <c r="A353" s="13">
         <v>3482.5165048543686</v>
       </c>
       <c r="B353" s="4">
         <v>75.682270872359368</v>
       </c>
       <c r="C353" s="4">
-        <v>94.411481799761333</v>
+        <v>83.293778159713611</v>
       </c>
       <c r="D353" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A354" s="3">
+      <c r="A354" s="13">
         <v>3483.0548543689315</v>
       </c>
       <c r="B354" s="4">
         <v>94.117494549086587</v>
       </c>
       <c r="C354" s="4">
-        <v>98.219957162272564</v>
+        <v>87.863948594727077</v>
       </c>
       <c r="D354" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A355" s="3">
+      <c r="A355" s="13">
         <v>3483.5932038834949</v>
       </c>
       <c r="B355" s="4">
         <v>102.73393150721456</v>
       </c>
       <c r="C355" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D355" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A356" s="3">
+      <c r="A356" s="13">
         <v>3484.1315533980578</v>
       </c>
       <c r="B356" s="4">
         <v>79.222338889618328</v>
       </c>
       <c r="C356" s="4">
-        <v>95.142813410473764</v>
+        <v>84.171376092568522</v>
       </c>
       <c r="D356" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A357" s="3">
+      <c r="A357" s="13">
         <v>3484.6699029126212</v>
       </c>
       <c r="B357" s="4">
         <v>58.115378998724374</v>
       </c>
       <c r="C357" s="4">
-        <v>90.782392396246451</v>
+        <v>78.938870875495752</v>
       </c>
       <c r="D357" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A358" s="3">
+      <c r="A358" s="13">
         <v>3485.2082524271841</v>
       </c>
       <c r="B358" s="4">
         <v>65.195588506906546</v>
       </c>
       <c r="C358" s="4">
-        <v>92.245070796366448</v>
+        <v>80.694084955639738</v>
       </c>
       <c r="D358" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A359" s="3">
+      <c r="A359" s="13">
         <v>3485.746601941747</v>
       </c>
       <c r="B359" s="4">
         <v>65.930311791162381</v>
       </c>
       <c r="C359" s="4">
-        <v>92.396854988162517</v>
+        <v>80.876225985795017</v>
       </c>
       <c r="D359" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A360" s="3">
+      <c r="A360" s="13">
         <v>3486.2849514563104</v>
       </c>
       <c r="B360" s="4">
         <v>43.687829777199482</v>
       </c>
       <c r="C360" s="4">
-        <v>87.801850000063823</v>
+        <v>75.362220000076576</v>
       </c>
       <c r="D360" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A361" s="3">
+      <c r="A361" s="13">
         <v>3486.8233009708733</v>
       </c>
       <c r="B361" s="4">
         <v>22.046515964048183</v>
       </c>
       <c r="C361" s="4">
-        <v>83.331038475611933</v>
+        <v>69.997246170734314</v>
       </c>
       <c r="D361" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A362" s="3">
+      <c r="A362" s="13">
         <v>3487.3616504854367</v>
       </c>
       <c r="B362" s="4">
         <v>-20.835386297105565</v>
       </c>
       <c r="C362" s="4">
-        <v>74.472200030088317</v>
+        <v>59.366640036105977</v>
       </c>
       <c r="D362" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A363" s="3">
+      <c r="A363" s="13">
         <v>3487.8999999999996</v>
       </c>
       <c r="B363" s="4">
         <v>-139.29498980595179</v>
       </c>
       <c r="C363" s="4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D363" s="2" t="s">
         <v>3</v>
@@ -7462,7 +7468,7 @@
   <dimension ref="A1:H130"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10671,7 +10677,7 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11175,31 +11181,31 @@
       <c r="R13" s="19"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="32">
         <v>2450</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="33">
         <v>0.03</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="33">
         <v>0.04</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="33">
         <v>0.09</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="33">
         <v>0.01</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="33">
         <v>0.17</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="33">
         <v>0.01</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="33">
         <v>0.82</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="35" t="s">
         <v>3</v>
       </c>
       <c r="J14" s="20"/>
@@ -11235,31 +11241,31 @@
       <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+      <c r="A16" s="42">
         <v>2475</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B16" s="43">
         <v>0.03</v>
       </c>
-      <c r="C16" s="33">
+      <c r="C16" s="43">
         <v>0.03</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="43">
         <v>0.06</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="43">
         <v>0.01</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="23">
         <v>0.13</v>
       </c>
-      <c r="G16" s="33">
-        <v>0</v>
-      </c>
-      <c r="H16" s="33">
+      <c r="G16" s="43">
+        <v>0</v>
+      </c>
+      <c r="H16" s="43">
         <v>0.87</v>
       </c>
-      <c r="I16" s="35" t="s">
+      <c r="I16" s="19" t="s">
         <v>3</v>
       </c>
       <c r="J16" s="20"/>

</xml_diff>

<commit_message>
changes on GR_core and CORE xls
</commit_message>
<xml_diff>
--- a/CORE/CORE.xlsx
+++ b/CORE/CORE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angelica\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FBD64B-BF5F-4CBF-B07D-6748C6983107}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B22ABD3-7920-493D-A7B1-B52F77F3685D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CF367FB8-77F3-451A-B253-26A736045F64}"/>
   </bookViews>
@@ -2845,7 +2845,7 @@
         <v>20.927710769465801</v>
       </c>
       <c r="C157" s="38">
-        <v>69.719889599830594</v>
+        <v>62.222472436770005</v>
       </c>
       <c r="D157" s="35" t="s">
         <v>3</v>
@@ -2859,7 +2859,7 @@
         <v>45.357685784253754</v>
       </c>
       <c r="C158" s="4">
-        <v>75.776184413418804</v>
+        <v>76.49038255548615</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>3</v>
@@ -2873,7 +2873,7 @@
         <v>60.58676588916471</v>
       </c>
       <c r="C159" s="4">
-        <v>79.55153820724226</v>
+        <v>85.384666974363753</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>3</v>
@@ -2887,7 +2887,7 @@
         <v>69.069634405000414</v>
       </c>
       <c r="C160" s="4">
-        <v>81.654477427020751</v>
+        <v>90.338941608683569</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>3</v>
@@ -2901,7 +2901,7 @@
         <v>68.334897761896528</v>
       </c>
       <c r="C161" s="4">
-        <v>81.472333085150154</v>
+        <v>89.909831207285777</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>3</v>
@@ -2915,7 +2915,7 @@
         <v>59.7184474449205</v>
       </c>
       <c r="C162" s="4">
-        <v>79.336278368161942</v>
+        <v>84.877540400988195</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>3</v>
@@ -2929,7 +2929,7 @@
         <v>54.241333100630548</v>
       </c>
       <c r="C163" s="4">
-        <v>77.978478404114753</v>
+        <v>81.678725210757506</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>3</v>
@@ -2943,7 +2943,7 @@
         <v>60.491213631037951</v>
       </c>
       <c r="C164" s="4">
-        <v>79.527850395651399</v>
+        <v>85.328861308178347</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>3</v>
@@ -2957,7 +2957,7 @@
         <v>59.765735154255026</v>
       </c>
       <c r="C165" s="4">
-        <v>79.348001192627208</v>
+        <v>84.905157980870968</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>3</v>
@@ -2971,7 +2971,7 @@
         <v>61.893879318115488</v>
       </c>
       <c r="C166" s="4">
-        <v>79.875577191143549</v>
+        <v>86.148064272475892</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>3</v>
@@ -2985,7 +2985,7 @@
         <v>77.018128960306655</v>
       </c>
       <c r="C167" s="4">
-        <v>83.624943066956774</v>
+        <v>94.981124248066763</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>3</v>
@@ -2999,7 +2999,7 @@
         <v>71.674609776005056</v>
       </c>
       <c r="C168" s="4">
-        <v>82.30026191183461</v>
+        <v>91.860333031821128</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>3</v>
@@ -3013,7 +3013,7 @@
         <v>57.247073913328236</v>
       </c>
       <c r="C169" s="4">
-        <v>78.723614348130752</v>
+        <v>83.434176852839329</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>3</v>
@@ -3027,7 +3027,7 @@
         <v>60.920743769999582</v>
       </c>
       <c r="C170" s="4">
-        <v>79.634332745768347</v>
+        <v>85.579721057820933</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>3</v>
@@ -3041,7 +3041,7 @@
         <v>56.77950087250499</v>
       </c>
       <c r="C171" s="4">
-        <v>78.60770100067964</v>
+        <v>83.161098795397095</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>3</v>
@@ -3055,7 +3055,7 @@
         <v>58.11539903699645</v>
       </c>
       <c r="C172" s="4">
-        <v>78.938875843068715</v>
+        <v>83.94130732721851</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>3</v>
@@ -3069,7 +3069,7 @@
         <v>62.790989177324391</v>
       </c>
       <c r="C173" s="4">
-        <v>80.097974544569283</v>
+        <v>86.672005980564379</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>3</v>
@@ -3083,7 +3083,7 @@
         <v>63.191767977865467</v>
       </c>
       <c r="C174" s="4">
-        <v>80.197329315486741</v>
+        <v>86.906074001515918</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>3</v>
@@ -3097,7 +3097,7 @@
         <v>53.640198296939069</v>
       </c>
       <c r="C175" s="4">
-        <v>77.829454527026854</v>
+        <v>81.327642684348433</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>3</v>
@@ -3111,7 +3111,7 @@
         <v>63.726121900122848</v>
       </c>
       <c r="C176" s="4">
-        <v>80.329797927756246</v>
+        <v>87.218154293441586</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>3</v>
@@ -3125,7 +3125,7 @@
         <v>62.724188257618195</v>
       </c>
       <c r="C177" s="4">
-        <v>80.081414312177941</v>
+        <v>86.632992043070033</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>3</v>
@@ -3139,7 +3139,7 @@
         <v>35.672520943338967</v>
       </c>
       <c r="C178" s="4">
-        <v>73.375190816033893</v>
+        <v>70.833927264333596</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>3</v>
@@ -3153,7 +3153,7 @@
         <v>22.714458366869884</v>
       </c>
       <c r="C179" s="4">
-        <v>70.1628319360712</v>
+        <v>63.26599188814734</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>3</v>
@@ -3167,7 +3167,7 @@
         <v>23.649584410244309</v>
       </c>
       <c r="C180" s="4">
-        <v>70.394653663400504</v>
+        <v>63.812136300020896</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>3</v>
@@ -3181,7 +3181,7 @@
         <v>53.373021335810371</v>
       </c>
       <c r="C181" s="4">
-        <v>77.763220220892094</v>
+        <v>81.171602538385599</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>3</v>
@@ -3195,7 +3195,7 @@
         <v>69.537227484095723</v>
       </c>
       <c r="C182" s="4">
-        <v>81.770395742044826</v>
+        <v>90.612031369136744</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>3</v>
@@ -3209,7 +3209,7 @@
         <v>66.33109727112749</v>
       </c>
       <c r="C183" s="4">
-        <v>80.975582412570105</v>
+        <v>88.739545716579144</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>3</v>
@@ -3223,7 +3223,7 @@
         <v>56.044770908825129</v>
       </c>
       <c r="C184" s="4">
-        <v>78.425558314666702</v>
+        <v>82.731992295002954</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>3</v>
@@ -3237,7 +3237,7 @@
         <v>52.103917411601081</v>
       </c>
       <c r="C185" s="4">
-        <v>77.448603955036702</v>
+        <v>80.430404043054878</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>3</v>
@@ -3251,7 +3251,7 @@
         <v>52.571463734728219</v>
       </c>
       <c r="C186" s="4">
-        <v>77.564510679057221</v>
+        <v>80.70346649648252</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>3</v>
@@ -3265,7 +3265,7 @@
         <v>53.840554300089458</v>
       </c>
       <c r="C187" s="4">
-        <v>77.87912363319731</v>
+        <v>81.444657189805952</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>3</v>
@@ -3279,7 +3279,7 @@
         <v>52.838660734128986</v>
       </c>
       <c r="C188" s="4">
-        <v>77.630749952764944</v>
+        <v>80.859518345456308</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>3</v>
@@ -3293,7 +3293,7 @@
         <v>57.8482287552918</v>
       </c>
       <c r="C189" s="4">
-        <v>78.872643192791614</v>
+        <v>83.785271082259342</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>3</v>
@@ -3307,7 +3307,7 @@
         <v>57.447443275326691</v>
       </c>
       <c r="C190" s="4">
-        <v>78.773286766016525</v>
+        <v>83.551199160304151</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>3</v>
@@ -3321,7 +3321,7 @@
         <v>55.911175748836762</v>
       </c>
       <c r="C191" s="4">
-        <v>78.392439505741663</v>
+        <v>82.653968321017885</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>3</v>
@@ -3335,7 +3335,7 @@
         <v>54.976076423158453</v>
       </c>
       <c r="C192" s="4">
-        <v>78.160624401842995</v>
+        <v>82.107839513158922</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>3</v>
@@ -3349,7 +3349,7 @@
         <v>55.577231265122009</v>
       </c>
       <c r="C193" s="4">
-        <v>78.309653246503842</v>
+        <v>82.458933742578949</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>3</v>
@@ -3363,7 +3363,7 @@
         <v>56.979910311047604</v>
       </c>
       <c r="C194" s="4">
-        <v>78.65738335371131</v>
+        <v>83.278144508883798</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>3</v>
@@ -3377,7 +3377,7 @@
         <v>60.920763808271658</v>
       </c>
       <c r="C195" s="4">
-        <v>79.634337713341296</v>
+        <v>85.579732760831874</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>3</v>
@@ -3391,7 +3391,7 @@
         <v>60.186007126895696</v>
       </c>
       <c r="C196" s="4">
-        <v>79.452188403897765</v>
+        <v>85.15061065642314</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>3</v>
@@ -3405,7 +3405,7 @@
         <v>52.304286773599529</v>
       </c>
       <c r="C197" s="4">
-        <v>77.498276372922462</v>
+        <v>80.5474263505197</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>3</v>
@@ -3419,7 +3419,7 @@
         <v>55.844394867402649</v>
       </c>
       <c r="C198" s="4">
-        <v>78.375884240923284</v>
+        <v>82.61496608653448</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>3</v>
@@ -3433,7 +3433,7 @@
         <v>52.237499212741398</v>
       </c>
       <c r="C199" s="4">
-        <v>77.481719452246438</v>
+        <v>80.508420215032643</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>3</v>
@@ -3447,7 +3447,7 @@
         <v>54.441715821477068</v>
       </c>
       <c r="C200" s="4">
-        <v>78.028154133715816</v>
+        <v>81.795755320229631</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>3</v>
@@ -3461,7 +3461,7 @@
         <v>63.659307621568601</v>
       </c>
       <c r="C201" s="4">
-        <v>80.313234383649586</v>
+        <v>87.179132553939922</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>3</v>
@@ -3475,7 +3475,7 @@
         <v>71.006674052607394</v>
       </c>
       <c r="C202" s="4">
-        <v>82.134677802355384</v>
+        <v>91.470236567917709</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>3</v>
@@ -3489,7 +3489,7 @@
         <v>66.26430303084534</v>
       </c>
       <c r="C203" s="4">
-        <v>80.959023836036422</v>
+        <v>88.70053568008845</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>3</v>
@@ -3503,7 +3503,7 @@
         <v>61.922677412504228</v>
       </c>
       <c r="C204" s="4">
-        <v>79.882716361346638</v>
+        <v>86.164883308192486</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>3</v>
@@ -3517,7 +3517,7 @@
         <v>56.645912391940648</v>
       </c>
       <c r="C205" s="4">
-        <v>78.574583847612246</v>
+        <v>83.083078722415678</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>3</v>
@@ -3531,7 +3531,7 @@
         <v>49.832893203735175</v>
       </c>
       <c r="C206" s="4">
-        <v>76.885607385318309</v>
+        <v>79.104051099359879</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>3</v>
@@ -3545,7 +3545,7 @@
         <v>46.29279846878012</v>
       </c>
       <c r="C207" s="4">
-        <v>76.008002829032804</v>
+        <v>77.036519165352402</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>3</v>
@@ -3559,7 +3559,7 @@
         <v>44.890119422854539</v>
       </c>
       <c r="C208" s="4">
-        <v>75.660272721825336</v>
+        <v>76.217308399047553</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>3</v>
@@ -3573,7 +3573,7 @@
         <v>52.972229176421251</v>
       </c>
       <c r="C209" s="4">
-        <v>77.663862138259361</v>
+        <v>80.93752671542677</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>3</v>
@@ -3587,7 +3587,7 @@
         <v>56.979896952199553</v>
       </c>
       <c r="C210" s="4">
-        <v>78.657380041996007</v>
+        <v>83.278136706876495</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>3</v>
@@ -3601,7 +3601,7 @@
         <v>62.123040095078657</v>
       </c>
       <c r="C211" s="4">
-        <v>79.932387123374752</v>
+        <v>86.281901714653657</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>3</v>
@@ -3615,7 +3615,7 @@
         <v>59.317675323803449</v>
       </c>
       <c r="C212" s="4">
-        <v>79.236925253102157</v>
+        <v>84.643476281040307</v>
       </c>
       <c r="D212" s="2" t="s">
         <v>3</v>
@@ -3629,7 +3629,7 @@
         <v>53.372987938690244</v>
       </c>
       <c r="C213" s="4">
-        <v>77.763211941603828</v>
+        <v>81.171583033367369</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>3</v>
@@ -3643,7 +3643,7 @@
         <v>55.643998787708071</v>
       </c>
       <c r="C214" s="4">
-        <v>78.326205199606918</v>
+        <v>82.497928175055051</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>3</v>
@@ -3657,7 +3657,7 @@
         <v>55.844394867402642</v>
       </c>
       <c r="C215" s="4">
-        <v>78.375884240923284</v>
+        <v>82.61496608653448</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>3</v>
@@ -3671,7 +3671,7 @@
         <v>53.9741427806538</v>
       </c>
       <c r="C216" s="4">
-        <v>77.91224078626469</v>
+        <v>81.522677262787369</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>3</v>
@@ -3685,7 +3685,7 @@
         <v>53.573377338960782</v>
       </c>
       <c r="C217" s="4">
-        <v>77.81288932706255</v>
+        <v>81.288617043843132</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>3</v>
@@ -3699,7 +3699,7 @@
         <v>58.31578175784297</v>
       </c>
       <c r="C218" s="4">
-        <v>78.988551572669792</v>
+        <v>84.058337436690636</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>3</v>
@@ -3713,7 +3713,7 @@
         <v>69.336811366129098</v>
       </c>
       <c r="C219" s="4">
-        <v>81.720711733155497</v>
+        <v>90.494981754646403</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>3</v>
@@ -3727,7 +3727,7 @@
         <v>78.487602246514442</v>
       </c>
       <c r="C220" s="4">
-        <v>83.98923175069794</v>
+        <v>95.839345050862335</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>3</v>
@@ -3741,7 +3741,7 @@
         <v>69.537187407551585</v>
       </c>
       <c r="C221" s="4">
-        <v>81.770385806898929</v>
+        <v>90.612007963114877</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>3</v>
@@ -3755,7 +3755,7 @@
         <v>68.134515041050037</v>
       </c>
       <c r="C222" s="4">
-        <v>81.42265735554912</v>
+        <v>89.79280109781368</v>
       </c>
       <c r="D222" s="2" t="s">
         <v>3</v>
@@ -3769,7 +3769,7 @@
         <v>76.149823874910538</v>
       </c>
       <c r="C223" s="4">
-        <v>83.409686539591775</v>
+        <v>94.474005476698537</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>3</v>
@@ -3783,7 +3783,7 @@
         <v>81.092597655791167</v>
       </c>
       <c r="C224" s="4">
-        <v>84.635021203084762</v>
+        <v>97.360748177010848</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>3</v>
@@ -3797,7 +3797,7 @@
         <v>85.100252072721446</v>
       </c>
       <c r="C225" s="4">
-        <v>85.628535795106117</v>
+        <v>99.701350366453298</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>3</v>
@@ -3811,7 +3811,7 @@
         <v>94.31786391108507</v>
       </c>
       <c r="C226" s="4">
-        <v>87.91362101261285</v>
+        <v>105.08473930317454</v>
       </c>
       <c r="D226" s="2" t="s">
         <v>3</v>
@@ -3825,7 +3825,7 @@
         <v>79.689938648137669</v>
       </c>
       <c r="C227" s="4">
-        <v>84.28729606345027</v>
+        <v>96.541549113716954</v>
       </c>
       <c r="D227" s="2" t="s">
         <v>3</v>
@@ -3839,7 +3839,7 @@
         <v>80.491462852099701</v>
       </c>
       <c r="C228" s="4">
-        <v>84.485997325996863</v>
+        <v>97.009665650601789</v>
       </c>
       <c r="D228" s="2" t="s">
         <v>3</v>
@@ -3853,7 +3853,7 @@
         <v>73.745251263024457</v>
       </c>
       <c r="C229" s="4">
-        <v>82.813582751951941</v>
+        <v>93.069655866044002</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>3</v>
@@ -3867,7 +3867,7 @@
         <v>70.271937409503522</v>
       </c>
       <c r="C230" s="4">
-        <v>81.952533460484801</v>
+        <v>91.041126166519945</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>3</v>
@@ -3881,7 +3881,7 @@
         <v>70.806284652336856</v>
       </c>
       <c r="C231" s="4">
-        <v>82.085000416896662</v>
+        <v>91.353202557441946</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>3</v>
@@ -3895,7 +3895,7 @@
         <v>78.821593486197372</v>
       </c>
       <c r="C232" s="4">
-        <v>84.072029600939345</v>
+        <v>96.034406936326818</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>3</v>
@@ -3909,7 +3909,7 @@
         <v>84.499103910181901</v>
       </c>
       <c r="C233" s="4">
-        <v>85.479508606302915</v>
+        <v>99.350260038036936</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>3</v>
@@ -3923,7 +3923,7 @@
         <v>80.291066772405117</v>
       </c>
       <c r="C234" s="4">
-        <v>84.436318284680496</v>
+        <v>96.892627739122361</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>3</v>
@@ -3937,7 +3937,7 @@
         <v>82.762453662845445</v>
       </c>
       <c r="C235" s="4">
-        <v>85.04898561642699</v>
+        <v>98.335999089278545</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>3</v>
@@ -3951,7 +3951,7 @@
         <v>84.833075111592763</v>
       </c>
       <c r="C236" s="4">
-        <v>85.562301488971357</v>
+        <v>99.545310220490478</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>3</v>
@@ -3965,7 +3965,7 @@
         <v>87.772021684008294</v>
       </c>
       <c r="C237" s="4">
-        <v>86.290878856453674</v>
+        <v>101.26175182608159</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>3</v>
@@ -3979,7 +3979,7 @@
         <v>76.817772957156279</v>
       </c>
       <c r="C238" s="4">
-        <v>83.575273960786319</v>
+        <v>94.864109742609259</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>3</v>
@@ -3993,7 +3993,7 @@
         <v>53.172625256115815</v>
       </c>
       <c r="C239" s="4">
-        <v>77.713541179575742</v>
+        <v>81.054564626906199</v>
       </c>
       <c r="D239" s="2" t="s">
         <v>3</v>
@@ -4007,7 +4007,7 @@
         <v>41.149655325901008</v>
       </c>
       <c r="C240" s="4">
-        <v>74.732995747654059</v>
+        <v>74.032754157575241</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>3</v>
@@ -4021,7 +4021,7 @@
         <v>48.096269674094842</v>
       </c>
       <c r="C241" s="4">
-        <v>76.45509101887302</v>
+        <v>78.089805754616094</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>3</v>
@@ -4035,7 +4035,7 @@
         <v>47.5619224312615</v>
       </c>
       <c r="C242" s="4">
-        <v>76.322624062461159</v>
+        <v>77.777729363694078</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>3</v>
@@ -4049,7 +4049,7 @@
         <v>43.487467094625039</v>
       </c>
       <c r="C243" s="4">
-        <v>75.312549238048462</v>
+        <v>75.398113236757283</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>3</v>
@@ -4063,7 +4063,7 @@
         <v>57.313854794762335</v>
       </c>
       <c r="C244" s="4">
-        <v>78.740169612949131</v>
+        <v>83.473179087322734</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>3</v>
@@ -4077,7 +4077,7 @@
         <v>63.726101861850751</v>
       </c>
       <c r="C245" s="4">
-        <v>80.329792960183283</v>
+        <v>87.218142590430631</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>3</v>
@@ -4091,7 +4091,7 @@
         <v>57.781434515009622</v>
       </c>
       <c r="C246" s="4">
-        <v>78.856084616257917</v>
+        <v>83.74626104576862</v>
       </c>
       <c r="D246" s="2" t="s">
         <v>3</v>
@@ -4105,7 +4105,7 @@
         <v>48.630623596352216</v>
       </c>
       <c r="C247" s="4">
-        <v>76.58755963114254</v>
+        <v>78.401886046541748</v>
       </c>
       <c r="D247" s="2" t="s">
         <v>3</v>
@@ -4119,7 +4119,7 @@
         <v>36.474058506149056</v>
       </c>
       <c r="C248" s="4">
-        <v>73.573895390295831</v>
+        <v>71.302051603225749</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>3</v>
@@ -4133,7 +4133,7 @@
         <v>34.603826457672298</v>
       </c>
       <c r="C249" s="4">
-        <v>73.1102569032102</v>
+        <v>70.209774482489593</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>3</v>
@@ -4147,7 +4147,7 @@
         <v>46.760364830179348</v>
       </c>
       <c r="C250" s="4">
-        <v>76.123914520626272</v>
+        <v>77.309593321790999</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>3</v>
@@ -4161,7 +4161,7 @@
         <v>46.426386949344462</v>
       </c>
       <c r="C251" s="4">
-        <v>76.041119982100184</v>
+        <v>77.114539238333819</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>3</v>
@@ -4175,7 +4175,7 @@
         <v>32.867156172063758</v>
       </c>
       <c r="C252" s="4">
-        <v>72.679728945761312</v>
+        <v>69.195501830720247</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>3</v>
@@ -4189,7 +4189,7 @@
         <v>26.788880306386197</v>
       </c>
       <c r="C253" s="4">
-        <v>71.172898481195617</v>
+        <v>65.645588510065892</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>3</v>
@@ -4203,7 +4203,7 @@
         <v>24.117110695099363</v>
       </c>
       <c r="C254" s="4">
-        <v>70.51055541984806</v>
+        <v>64.085187050437597</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>3</v>
@@ -4217,7 +4217,7 @@
         <v>37.542752991815732</v>
       </c>
       <c r="C255" s="4">
-        <v>73.838829303119553</v>
+        <v>71.926204385069752</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>3</v>
@@ -4231,7 +4231,7 @@
         <v>57.914996277877869</v>
       </c>
       <c r="C256" s="4">
-        <v>78.889195145894689</v>
+        <v>83.824265514735458</v>
       </c>
       <c r="D256" s="2" t="s">
         <v>3</v>
@@ -4245,7 +4245,7 @@
         <v>55.577204547425914</v>
       </c>
       <c r="C257" s="4">
-        <v>78.30964662307322</v>
+        <v>82.458918138564357</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>3</v>
@@ -4259,7 +4259,7 @@
         <v>44.288991298587078</v>
       </c>
       <c r="C258" s="4">
-        <v>75.511250500595082</v>
+        <v>75.866229773642132</v>
       </c>
       <c r="D258" s="2" t="s">
         <v>3</v>
@@ -4273,7 +4273,7 @@
         <v>42.819511332955287</v>
       </c>
       <c r="C259" s="4">
-        <v>75.146960160996287</v>
+        <v>75.008005069842923</v>
       </c>
       <c r="D259" s="2" t="s">
         <v>3</v>
@@ -4287,7 +4287,7 @@
         <v>42.552341051250629</v>
       </c>
       <c r="C260" s="4">
-        <v>75.080727510719186</v>
+        <v>74.851968824883741</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>3</v>
@@ -4301,7 +4301,7 @@
         <v>47.02754847073205</v>
       </c>
       <c r="C261" s="4">
-        <v>76.190150482618691</v>
+        <v>77.46563736875747</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>3</v>
@@ -4315,7 +4315,7 @@
         <v>35.271768860493992</v>
       </c>
       <c r="C262" s="4">
-        <v>73.275842668547071</v>
+        <v>70.599874847396649</v>
       </c>
       <c r="D262" s="2" t="s">
         <v>3</v>
@@ -4329,7 +4329,7 @@
         <v>41.884385289580869</v>
       </c>
       <c r="C263" s="4">
-        <v>74.915138433666982</v>
+        <v>74.461860657969368</v>
       </c>
       <c r="D263" s="2" t="s">
         <v>3</v>
@@ -4343,7 +4343,7 @@
         <v>48.163037196680918</v>
       </c>
       <c r="C264" s="4">
-        <v>76.471642971976109</v>
+        <v>78.12880018709221</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>3</v>
@@ -4357,7 +4357,7 @@
         <v>35.739308504197119</v>
       </c>
       <c r="C265" s="4">
-        <v>73.391747736709931</v>
+        <v>70.872933399820667</v>
       </c>
       <c r="D265" s="2" t="s">
         <v>3</v>
@@ -4371,7 +4371,7 @@
         <v>33.468311014027329</v>
       </c>
       <c r="C266" s="4">
-        <v>72.828757790422173</v>
+        <v>69.54659606014026</v>
       </c>
       <c r="D266" s="2" t="s">
         <v>3</v>
@@ -4385,7 +4385,7 @@
         <v>49.632530521160746</v>
       </c>
       <c r="C267" s="4">
-        <v>76.835936623290195</v>
+        <v>78.987032692898708</v>
       </c>
       <c r="D267" s="2" t="s">
         <v>3</v>
@@ -4399,7 +4399,7 @@
         <v>70.138348928939166</v>
       </c>
       <c r="C268" s="4">
-        <v>81.919416307417421</v>
+        <v>90.963106093538528</v>
       </c>
       <c r="D268" s="2" t="s">
         <v>3</v>
@@ -4413,7 +4413,7 @@
         <v>71.140255853747689</v>
       </c>
       <c r="C269" s="4">
-        <v>82.167793299565119</v>
+        <v>91.548252739895474</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>3</v>
@@ -4427,7 +4427,7 @@
         <v>58.382555959853065</v>
       </c>
       <c r="C270" s="4">
-        <v>79.005105181630512</v>
+        <v>84.097335770170403</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>3</v>
@@ -4441,7 +4441,7 @@
         <v>49.766098963453004</v>
       </c>
       <c r="C271" s="4">
-        <v>76.86904880878464</v>
+        <v>79.06504106286917</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>3</v>
@@ -4455,7 +4455,7 @@
         <v>33.267928293180809</v>
       </c>
       <c r="C272" s="4">
-        <v>72.779082060821096</v>
+        <v>69.429565950668135</v>
       </c>
       <c r="D272" s="2" t="s">
         <v>3</v>
@@ -4469,7 +4469,7 @@
         <v>27.189665786351316</v>
       </c>
       <c r="C273" s="4">
-        <v>71.272254907970705</v>
+        <v>65.879660432021083</v>
       </c>
       <c r="D273" s="2" t="s">
         <v>3</v>
@@ -4483,7 +4483,7 @@
         <v>40.8824716853483</v>
       </c>
       <c r="C274" s="4">
-        <v>74.66675978566164</v>
+        <v>73.876710110608769</v>
       </c>
       <c r="D274" s="2" t="s">
         <v>3</v>
@@ -4497,7 +4497,7 @@
         <v>54.040930341511945</v>
       </c>
       <c r="C275" s="4">
-        <v>77.928797706940728</v>
+        <v>81.561683398274425</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>3</v>
@@ -4511,7 +4511,7 @@
         <v>62.523798857347664</v>
       </c>
       <c r="C276" s="4">
-        <v>80.031736926719219</v>
+        <v>86.515958032594256</v>
       </c>
       <c r="D276" s="2" t="s">
         <v>3</v>
@@ -4525,7 +4525,7 @@
         <v>66.264276313149239</v>
       </c>
       <c r="C277" s="4">
-        <v>80.959017212605815</v>
+        <v>88.700520076073872</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>3</v>
@@ -4539,7 +4539,7 @@
         <v>72.676530059661673</v>
       </c>
       <c r="C278" s="4">
-        <v>82.548642215697612</v>
+        <v>92.445487480185392</v>
       </c>
       <c r="D278" s="2" t="s">
         <v>3</v>
@@ -4553,7 +4553,7 @@
         <v>67.600181157064711</v>
       </c>
       <c r="C279" s="4">
-        <v>81.290193710852549</v>
+        <v>89.480732508898939</v>
       </c>
       <c r="D279" s="2" t="s">
         <v>3</v>
@@ -4567,7 +4567,7 @@
         <v>63.859690342415092</v>
       </c>
       <c r="C280" s="4">
-        <v>80.362910113250649</v>
+        <v>87.296162663412048</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>3</v>
@@ -4581,7 +4581,7 @@
         <v>74.413173627574096</v>
       </c>
       <c r="C281" s="4">
-        <v>82.979163549715878</v>
+        <v>93.459744527940146</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>3</v>
@@ -4595,7 +4595,7 @@
         <v>65.930305111738377</v>
       </c>
       <c r="C282" s="4">
-        <v>80.876224329937372</v>
+        <v>88.505469893620329</v>
       </c>
       <c r="D282" s="2" t="s">
         <v>3</v>
@@ -4609,7 +4609,7 @@
         <v>64.460831825530619</v>
       </c>
       <c r="C283" s="4">
-        <v>80.511935646196207</v>
+        <v>87.647249090824772</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>3</v>
@@ -4623,7 +4623,7 @@
         <v>64.460831825530619</v>
       </c>
       <c r="C284" s="4">
-        <v>80.511935646196207</v>
+        <v>87.647249090824772</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>3</v>
@@ -4637,7 +4637,7 @@
         <v>64.527626065812768</v>
       </c>
       <c r="C285" s="4">
-        <v>80.528494222729904</v>
+        <v>87.686259127315452</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>3</v>
@@ -4651,7 +4651,7 @@
         <v>70.605908610914355</v>
       </c>
       <c r="C286" s="4">
-        <v>82.035326343153244</v>
+        <v>91.236176348973459</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>3</v>
@@ -4665,7 +4665,7 @@
         <v>68.201335999028302</v>
       </c>
       <c r="C287" s="4">
-        <v>81.439222555513396</v>
+        <v>89.831826738318966</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>3</v>
@@ -4679,7 +4679,7 @@
         <v>66.932245433667035</v>
       </c>
       <c r="C288" s="4">
-        <v>81.124609601373322</v>
+        <v>89.090636044995506</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>3</v>
@@ -4693,7 +4693,7 @@
         <v>63.525719141004252</v>
       </c>
       <c r="C289" s="4">
-        <v>80.280117230582221</v>
+        <v>87.101112480958506</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>3</v>
@@ -4707,7 +4707,7 @@
         <v>61.121119811422069</v>
       </c>
       <c r="C290" s="4">
-        <v>79.684006819511751</v>
+        <v>85.696747266289407</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>3</v>
@@ -4721,7 +4721,7 @@
         <v>66.063893592302719</v>
       </c>
       <c r="C291" s="4">
-        <v>80.909341483004738</v>
+        <v>88.583489966601732</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>3</v>
@@ -4735,7 +4735,7 @@
         <v>75.28149875124231</v>
       </c>
       <c r="C292" s="4">
-        <v>83.194425044653826</v>
+        <v>93.966875002319341</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>3</v>
@@ -4749,7 +4749,7 @@
         <v>73.878819705316729</v>
       </c>
       <c r="C293" s="4">
-        <v>82.846694937446358</v>
+        <v>93.147664236014492</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>3</v>
@@ -4763,7 +4763,7 @@
         <v>55.911169069412743</v>
       </c>
       <c r="C294" s="4">
-        <v>78.392437849884033</v>
+        <v>82.653964420014233</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>3</v>
@@ -4777,7 +4777,7 @@
         <v>44.95691366313671</v>
       </c>
       <c r="C295" s="4">
-        <v>75.676831298359019</v>
+        <v>76.256318435538262</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>3</v>
@@ -4791,7 +4791,7 @@
         <v>46.626776349615007</v>
       </c>
       <c r="C296" s="4">
-        <v>76.090797367558906</v>
+        <v>77.231573248809582</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>3</v>
@@ -4805,7 +4805,7 @@
         <v>55.644018825980154</v>
       </c>
       <c r="C297" s="4">
-        <v>78.32621016717988</v>
+        <v>82.497939878066006</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>3</v>
@@ -4819,7 +4819,7 @@
         <v>57.313874833034426</v>
       </c>
       <c r="C298" s="4">
-        <v>78.740174580522094</v>
+        <v>83.473190790333689</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>3</v>
@@ -4833,7 +4833,7 @@
         <v>46.827165749885538</v>
       </c>
       <c r="C299" s="4">
-        <v>76.140474753017614</v>
+        <v>77.348607259285345</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>3</v>
@@ -4847,7 +4847,7 @@
         <v>24.785073136193159</v>
       </c>
       <c r="C300" s="4">
-        <v>70.676146152757894</v>
+        <v>64.475299118355622</v>
       </c>
       <c r="D300" s="2" t="s">
         <v>3</v>
@@ -4861,7 +4861,7 @@
         <v>23.582770131690058</v>
       </c>
       <c r="C301" s="4">
-        <v>70.378090119293859</v>
+        <v>63.773114560519247</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>3</v>
@@ -4875,7 +4875,7 @@
         <v>46.893973349015774</v>
       </c>
       <c r="C302" s="4">
-        <v>76.157036641266615</v>
+        <v>77.387625097783356</v>
       </c>
       <c r="D302" s="2" t="s">
         <v>3</v>
@@ -4889,7 +4889,7 @@
         <v>59.65167324291042</v>
       </c>
       <c r="C303" s="4">
-        <v>79.319724759201222</v>
+        <v>84.838542067508442</v>
       </c>
       <c r="D303" s="2" t="s">
         <v>3</v>
@@ -4903,7 +4903,7 @@
         <v>60.119219566037565</v>
       </c>
       <c r="C304" s="4">
-        <v>79.435631483221727</v>
+        <v>85.111604520936083</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>3</v>
@@ -4917,7 +4917,7 @@
         <v>42.752730451521167</v>
       </c>
       <c r="C305" s="4">
-        <v>75.130404896177893</v>
+        <v>74.969002835359504</v>
       </c>
       <c r="D305" s="2" t="s">
         <v>3</v>
@@ -4931,7 +4931,7 @@
         <v>37.876750910922695</v>
       </c>
       <c r="C306" s="4">
-        <v>73.921628809218603</v>
+        <v>72.121270171537887</v>
       </c>
       <c r="D306" s="2" t="s">
         <v>3</v>
@@ -4945,7 +4945,7 @@
         <v>36.340463346160682</v>
       </c>
       <c r="C307" s="4">
-        <v>73.540776581370793</v>
+        <v>71.22402762924068</v>
       </c>
       <c r="D307" s="2" t="s">
         <v>3</v>
@@ -4959,7 +4959,7 @@
         <v>36.60763362786534</v>
       </c>
       <c r="C308" s="4">
-        <v>73.607009231647908</v>
+        <v>71.380063874199863</v>
       </c>
       <c r="D308" s="2" t="s">
         <v>3</v>
@@ -4973,7 +4973,7 @@
         <v>42.819504653531261</v>
       </c>
       <c r="C309" s="4">
-        <v>75.146958505138628</v>
+        <v>75.008001168839272</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>3</v>
@@ -4987,7 +4987,7 @@
         <v>40.481726281927358</v>
       </c>
       <c r="C310" s="4">
-        <v>74.567413294032463</v>
+        <v>73.642661594675474</v>
       </c>
       <c r="D310" s="2" t="s">
         <v>3</v>
@@ -5001,7 +5001,7 @@
         <v>40.615314762491707</v>
       </c>
       <c r="C311" s="4">
-        <v>74.600530447099857</v>
+        <v>73.720681667656891</v>
       </c>
       <c r="D311" s="2" t="s">
         <v>3</v>
@@ -5015,7 +5015,7 @@
         <v>41.216449566183186</v>
       </c>
       <c r="C312" s="4">
-        <v>74.749554324187756</v>
+        <v>74.071764194065949</v>
       </c>
       <c r="D312" s="2" t="s">
         <v>3</v>
@@ -5029,7 +5029,7 @@
         <v>44.689756740280103</v>
       </c>
       <c r="C313" s="4">
-        <v>75.610601959797236</v>
+        <v>76.100289992586369</v>
       </c>
       <c r="D313" s="2" t="s">
         <v>3</v>
@@ -5043,7 +5043,7 @@
         <v>49.432141120890215</v>
       </c>
       <c r="C314" s="4">
-        <v>76.786259237831487</v>
+        <v>78.869998682422931</v>
       </c>
       <c r="D314" s="2" t="s">
         <v>3</v>
@@ -5057,7 +5057,7 @@
         <v>53.439808896668524</v>
       </c>
       <c r="C315" s="4">
-        <v>77.779777141568132</v>
+        <v>81.21060867387267</v>
       </c>
       <c r="D315" s="2" t="s">
         <v>3</v>
@@ -5071,7 +5071,7 @@
         <v>60.787175327707317</v>
       </c>
       <c r="C316" s="4">
-        <v>79.60122056027393</v>
+        <v>85.501712687850457</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>3</v>
@@ -5085,7 +5085,7 @@
         <v>69.603995006681799</v>
       </c>
       <c r="C317" s="4">
-        <v>81.786947695147916</v>
+        <v>90.65102580161286</v>
       </c>
       <c r="D317" s="2" t="s">
         <v>3</v>
@@ -5099,7 +5099,7 @@
         <v>63.99327214355543</v>
       </c>
       <c r="C318" s="4">
-        <v>80.396025610460384</v>
+        <v>87.374178835389813</v>
       </c>
       <c r="D318" s="2" t="s">
         <v>3</v>
@@ -5113,7 +5113,7 @@
         <v>58.582938680699577</v>
       </c>
       <c r="C319" s="4">
-        <v>79.054780911231575</v>
+        <v>84.214365879642529</v>
       </c>
       <c r="D319" s="2" t="s">
         <v>3</v>
@@ -5127,7 +5127,7 @@
         <v>63.792889422708903</v>
       </c>
       <c r="C320" s="4">
-        <v>80.346349880859322</v>
+        <v>87.257148725917688</v>
       </c>
       <c r="D320" s="2" t="s">
         <v>3</v>
@@ -5141,7 +5141,7 @@
         <v>62.323422815925163</v>
       </c>
       <c r="C321" s="4">
-        <v>79.982062852975815</v>
+        <v>86.398931824125782</v>
       </c>
       <c r="D321" s="2" t="s">
         <v>3</v>
@@ -5155,7 +5155,7 @@
         <v>54.642105221747599</v>
       </c>
       <c r="C322" s="4">
-        <v>78.077831519174538</v>
+        <v>81.912789330705394</v>
       </c>
       <c r="D322" s="2" t="s">
         <v>3</v>
@@ -5169,7 +5169,7 @@
         <v>46.426420346464603</v>
       </c>
       <c r="C323" s="4">
-        <v>76.041128261388451</v>
+        <v>77.114558743352063</v>
       </c>
       <c r="D323" s="2" t="s">
         <v>3</v>
@@ -5183,7 +5183,7 @@
         <v>51.569570168767733</v>
       </c>
       <c r="C324" s="4">
-        <v>77.316136998624842</v>
+        <v>80.118327652132862</v>
       </c>
       <c r="D324" s="2" t="s">
         <v>3</v>
@@ -5197,7 +5197,7 @@
         <v>51.970322251612707</v>
       </c>
       <c r="C325" s="4">
-        <v>77.415485146111678</v>
+        <v>80.35238006906981</v>
       </c>
       <c r="D325" s="2" t="s">
         <v>3</v>
@@ -5211,7 +5211,7 @@
         <v>62.857790097030602</v>
       </c>
       <c r="C326" s="4">
-        <v>80.114534776960639</v>
+        <v>86.711019918058739</v>
       </c>
       <c r="D326" s="2" t="s">
         <v>3</v>
@@ -5225,7 +5225,7 @@
         <v>68.134528399898073</v>
       </c>
       <c r="C327" s="4">
-        <v>81.42266066726441</v>
+        <v>89.792808899820955</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>3</v>
@@ -5239,7 +5239,7 @@
         <v>52.371101052153769</v>
       </c>
       <c r="C328" s="4">
-        <v>77.514839917029107</v>
+        <v>80.586448090021335</v>
       </c>
       <c r="D328" s="2" t="s">
         <v>3</v>
@@ -5253,7 +5253,7 @@
         <v>66.130714550280999</v>
       </c>
       <c r="C329" s="4">
-        <v>80.925906682969043</v>
+        <v>88.622515607107033</v>
       </c>
       <c r="D329" s="2" t="s">
         <v>3</v>
@@ -5267,7 +5267,7 @@
         <v>68.000939919333732</v>
       </c>
       <c r="C330" s="4">
-        <v>81.389543514197044</v>
+        <v>89.714788826839538</v>
       </c>
       <c r="D330" s="2" t="s">
         <v>3</v>
@@ -5281,7 +5281,7 @@
         <v>72.676543418509709</v>
       </c>
       <c r="C331" s="4">
-        <v>82.548645527412916</v>
+        <v>92.445495282192695</v>
       </c>
       <c r="D331" s="2" t="s">
         <v>3</v>
@@ -5295,7 +5295,7 @@
         <v>66.731842674548446</v>
       </c>
       <c r="C332" s="4">
-        <v>81.074928904199282</v>
+        <v>88.973594232512454</v>
       </c>
       <c r="D332" s="2" t="s">
         <v>3</v>
@@ -5309,7 +5309,7 @@
         <v>57.647825996173196</v>
       </c>
       <c r="C333" s="4">
-        <v>78.822962495617588</v>
+        <v>83.668229269776276</v>
       </c>
       <c r="D333" s="2" t="s">
         <v>3</v>
@@ -5323,7 +5323,7 @@
         <v>57.781427835585603</v>
       </c>
       <c r="C334" s="4">
-        <v>78.856082960400272</v>
+        <v>83.746257144764982</v>
       </c>
       <c r="D334" s="2" t="s">
         <v>3</v>
@@ -5337,7 +5337,7 @@
         <v>64.928404866353873</v>
       </c>
       <c r="C335" s="4">
-        <v>80.627848993647333</v>
+        <v>87.920327148267006</v>
       </c>
       <c r="D335" s="2" t="s">
         <v>3</v>
@@ -5351,7 +5351,7 @@
         <v>67.800570557335277</v>
       </c>
       <c r="C336" s="4">
-        <v>81.339871096311271</v>
+        <v>89.597766519374716</v>
       </c>
       <c r="D336" s="2" t="s">
         <v>3</v>
@@ -5365,7 +5365,7 @@
         <v>62.056272572492595</v>
       </c>
       <c r="C337" s="4">
-        <v>79.915835170271663</v>
+        <v>86.242907282177541</v>
       </c>
       <c r="D337" s="2" t="s">
         <v>3</v>
@@ -5379,7 +5379,7 @@
         <v>62.390237094479424</v>
       </c>
       <c r="C338" s="4">
-        <v>79.998626397082461</v>
+        <v>86.437953563627431</v>
       </c>
       <c r="D338" s="2" t="s">
         <v>3</v>
@@ -5393,7 +5393,7 @@
         <v>70.539114370632191</v>
       </c>
       <c r="C339" s="4">
-        <v>82.018767766619561</v>
+        <v>91.197166312482764</v>
       </c>
       <c r="D339" s="2" t="s">
         <v>3</v>
@@ -5407,7 +5407,7 @@
         <v>71.741404016287248</v>
       </c>
       <c r="C340" s="4">
-        <v>82.316820488368307</v>
+        <v>91.89934306831185</v>
       </c>
       <c r="D340" s="2" t="s">
         <v>3</v>
@@ -5421,7 +5421,7 @@
         <v>79.355954087878757</v>
       </c>
       <c r="C341" s="4">
-        <v>84.20449986906651</v>
+        <v>96.346491129256123</v>
       </c>
       <c r="D341" s="2" t="s">
         <v>3</v>
@@ -5435,7 +5435,7 @@
         <v>82.428502499706667</v>
       </c>
       <c r="C342" s="4">
-        <v>84.96619770133151</v>
+        <v>98.140960609835943</v>
       </c>
       <c r="D342" s="2" t="s">
         <v>3</v>
@@ -5449,7 +5449,7 @@
         <v>83.163232463386521</v>
       </c>
       <c r="C343" s="4">
-        <v>85.148340387344433</v>
+        <v>98.57006711023007</v>
       </c>
       <c r="D343" s="2" t="s">
         <v>3</v>
@@ -5463,7 +5463,7 @@
         <v>69.336831404401181</v>
       </c>
       <c r="C344" s="4">
-        <v>81.720716700728474</v>
+        <v>90.49499345765733</v>
       </c>
       <c r="D344" s="2" t="s">
         <v>3</v>
@@ -5477,7 +5477,7 @@
         <v>71.874992496851604</v>
       </c>
       <c r="C345" s="4">
-        <v>82.349937641435687</v>
+        <v>91.977363141293267</v>
       </c>
       <c r="D345" s="2" t="s">
         <v>3</v>
@@ -5491,7 +5491,7 @@
         <v>76.550562598907462</v>
       </c>
       <c r="C346" s="4">
-        <v>83.509031375363307</v>
+        <v>94.708050091628195</v>
       </c>
       <c r="D346" s="2" t="s">
         <v>3</v>
@@ -5505,7 +5505,7 @@
         <v>70.071521291536868</v>
       </c>
       <c r="C347" s="4">
-        <v>81.902849451595472</v>
+        <v>90.924076552029589</v>
       </c>
       <c r="D347" s="2" t="s">
         <v>3</v>
@@ -5519,7 +5519,7 @@
         <v>59.117285923532904</v>
       </c>
       <c r="C348" s="4">
-        <v>79.187247867643435</v>
+        <v>84.52644227056453</v>
       </c>
       <c r="D348" s="2" t="s">
         <v>3</v>
@@ -5533,7 +5533,7 @@
         <v>66.598247514560086</v>
       </c>
       <c r="C349" s="4">
-        <v>81.041810095274258</v>
+        <v>88.895570258527385</v>
       </c>
       <c r="D349" s="2" t="s">
         <v>3</v>
@@ -5547,7 +5547,7 @@
         <v>68.401685322754673</v>
       </c>
       <c r="C350" s="4">
-        <v>81.488890005826207</v>
+        <v>89.948837342772833</v>
       </c>
       <c r="D350" s="2" t="s">
         <v>3</v>
@@ -5561,7 +5561,7 @@
         <v>74.212770868455493</v>
       </c>
       <c r="C351" s="4">
-        <v>82.929482852541838</v>
+        <v>93.342702715457079</v>
       </c>
       <c r="D351" s="2" t="s">
         <v>3</v>
@@ -5575,7 +5575,7 @@
         <v>71.74139733686323</v>
       </c>
       <c r="C352" s="4">
-        <v>82.316818832510663</v>
+        <v>91.899339167308199</v>
       </c>
       <c r="D352" s="2" t="s">
         <v>3</v>
@@ -5589,7 +5589,7 @@
         <v>75.682270872359368</v>
       </c>
       <c r="C353" s="4">
-        <v>83.293778159713611</v>
+        <v>94.200939122267229</v>
       </c>
       <c r="D353" s="2" t="s">
         <v>3</v>
@@ -5603,7 +5603,7 @@
         <v>94.117494549086587</v>
       </c>
       <c r="C354" s="4">
-        <v>87.863948594727077</v>
+        <v>104.96771699570971</v>
       </c>
       <c r="D354" s="2" t="s">
         <v>3</v>
@@ -5617,7 +5617,7 @@
         <v>102.73393150721456</v>
       </c>
       <c r="C355" s="4">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D355" s="2" t="s">
         <v>3</v>
@@ -5631,7 +5631,7 @@
         <v>79.222338889618328</v>
       </c>
       <c r="C356" s="4">
-        <v>84.171376092568522</v>
+        <v>96.268455452260127</v>
       </c>
       <c r="D356" s="2" t="s">
         <v>3</v>
@@ -5645,7 +5645,7 @@
         <v>58.115378998724374</v>
       </c>
       <c r="C357" s="4">
-        <v>78.938870875495752</v>
+        <v>83.941295624207584</v>
       </c>
       <c r="D357" s="2" t="s">
         <v>3</v>
@@ -5659,7 +5659,7 @@
         <v>65.195588506906546</v>
       </c>
       <c r="C358" s="4">
-        <v>80.694084955639738</v>
+        <v>88.076371195233463</v>
       </c>
       <c r="D358" s="2" t="s">
         <v>3</v>
@@ -5673,7 +5673,7 @@
         <v>65.930311791162381</v>
       </c>
       <c r="C359" s="4">
-        <v>80.876225985795017</v>
+        <v>88.505473794623953</v>
       </c>
       <c r="D359" s="2" t="s">
         <v>3</v>
@@ -5687,7 +5687,7 @@
         <v>43.687829777199482</v>
       </c>
       <c r="C360" s="4">
-        <v>75.362220000076576</v>
+        <v>75.515131643218467</v>
       </c>
       <c r="D360" s="2" t="s">
         <v>3</v>
@@ -5701,7 +5701,7 @@
         <v>22.046515964048183</v>
       </c>
       <c r="C361" s="4">
-        <v>69.997246170734314</v>
+        <v>62.875891523240277</v>
       </c>
       <c r="D361" s="2" t="s">
         <v>3</v>
@@ -5715,7 +5715,7 @@
         <v>-20.835386297105565</v>
       </c>
       <c r="C362" s="4">
-        <v>59.366640036105977</v>
+        <v>37.831448096206238</v>
       </c>
       <c r="D362" s="2" t="s">
         <v>3</v>
@@ -5729,7 +5729,7 @@
         <v>-139.29498980595179</v>
       </c>
       <c r="C363" s="4">
-        <v>30</v>
+        <v>-31.352862347823034</v>
       </c>
       <c r="D363" s="2" t="s">
         <v>3</v>

</xml_diff>